<commit_message>
Adding comments and cataloging into Function_Description.xlsx
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="17930" windowHeight="10040"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="17930" windowHeight="10040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,12 +636,1148 @@
         </r>
       </text>
     </comment>
+    <comment ref="B14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% data.flux            : Differential number flux [m-2 s^-1 eV^-1] (Isotropic flux)
+% data.energyFlux  : Differential energy flux [eV m-2 sr-1 s-1 eV-1]
+% data.chi2           : Measures the deviation between the measured q and inverted q (q-A*flux)/qSigma
+% data.qInverted    : Production rate derived from the estimated flux - A*flux [m-3 s-1]
+% data.maxIter      : The maximum number of iterations before convergence
+% data.energyBin   : The energy values of each energy spectral bin [eV]
+% data.time           : Time vector [s]
+% data.alt             : Altitude [km]
+% data.A               : Energy deposition matrix [nH x nE] [eV m^-1]
+% data.qInput        : The production rate which was input to this function [m^-3 s^-1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% q                : Production rates [m^-3 s^-1]   [nHxnT]
+% alt              : Altitude [km]                          [nHx1]
+% time            : Time [matlab units]                 [1xnT]
+% energyBin    : Energy bin values [eV]              [nEx1]
+% DateNumBeg: Initial time 
+% DateNumEnd: Final time </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% Using altitude profiles of production rates and the maximum entropy inversion 
+% method to estimate the energy spectra.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% differenitalDirectionalNumFlux_equator : j(alpha, E) [1 / (m sr s eV)] 
+% pitchAngle                                      : [deg]
+% L                                                  : magnetic L-shell (r_eq/RE)
+% latitude                                          : [deg] </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% differentialDirectionalNumFlux_latitude : j(alpha_lambda, E) [1/ m sr s eV)]
+% pitchAngleAtLatitude                        : Pitch angle associated with
+%                                                      values of diff num flux
+% invariantLatitude                             : The invariant latitude of the point</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% q                 : production rate [m-3 s-1]
+% qTime          : time instances where q is estimated [s]
+% alpha           : Effective recombination coefficients 
+%                     used for the calculation [m^3 s^-1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% Ne                : Electron density [length(height) x length(time)] [m-3]
+% alt                : height vector [length(height) x 1] [km]
+% time              : time vector [1 x length(time)] [s]
+% mode            : Choose between the following calculations
+%                 '1': q = dn/dt + alpha*ne^2 (Default)
+%                 '2': q = alpha*ne^2 
+% alpha            : User defined effective recombination coefficients 
+%                      per altitude point [m^3 s^-1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% timeAvgData: Time averaged data [nEx1]
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% data: Any type of 2D time series data, exmaple: energyFlux [nExnT]
+% time: Time array [nTx1]
+% timeMin: Minimum time value in matlab units
+% timeMax: Maximum time value in matlab units</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% noParticles - no. of particles per Energy [eV-1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% energyBin  - Energy variable in [eV]
+% meanEnergy - Mean energy in [eV]
+% T  - Temperature in [kappa]
+% kappa  - Kappa (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% numberFlux  - Differential Number Flux [eV-1 cm-2 s-1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% energyBin   - Energy variable in [eV]
+% meanEnergy  - Mean energy in [eV]
+% T     - Temperature in [K]
+% kappa    - Kappa (unitless)
+% plasmaDensity - density of plasma [m-3]
+% m     - mass of plasma [kg] Also 1 eV/(cm s-1)^2  = 1.6E-15 kg!  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% h2 - plot handle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% data arranged beam-wise
+% magcoords - arranged non-beam-wise</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nithin Sivadas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">% beamNo      : The beam ID of all beams in the measurment
+% latitude    : Geographic latitude value of each measurement along beams
+%               at the altitude points specified
+% longitude   : Geographic longitude value of each measurement along beams
+%               at the altitude points specified
+% altitudeGrid: The default altitude (of beam 1) 
+%               or user specified altitude points
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% fileNameStr : [String] The path to HDF5 file which contains the PFISR data
+%
+% msrParameter: [String] - The name of the measurement parameter
+%               (specified in the HDF5 file) which you would like to
+%               extract from the HDF5 file (e.g. 'dpopl','popl')
+%               Default: Uncorrected electron density: 'popl'
+%               IMPORTANT- The parameter has to be expressed in log scale
+% altitudeGrid: [N x 1] [km] - A column vector of the altitude points for 
+%               which you need the 
+%               value of the measurement parameter 
+%               Default value of the altitude grid is the altitude projection 
+%               of the range points of the beam pointing along 
+%               the magnetic field line</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% msrParValue : The value of the measurement parameter per altitude; 
+%               Units as given by the HDF5 file
+% altitudeGrid: The default altitude (of beam 1) 
+%               or user specified altitude points
+% time        : Time array</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% fileNameStr : [String] The path to HDF5 file which contains the PFISR data
+%
+% msrParameter: [String] - The name of the measurement parameter
+%               (specified in the HDF5 file) which you would like to
+%               extract from the HDF5 file (e.g. 'dpopl','popl')
+%               Default: Uncorrected electron density: 'popl'
+%               IMPORTANT- The parameter has to be expressed in log scale
+% altitudeGrid: [N x 1] [km] - A column vector of the altitude points for 
+%               which you need the 
+%               value of the measurement parameter 
+%               Default value of the altitude grid is the altitude projection 
+%               of the range points of the beam pointing along 
+%               the magnetic field line
+% mode        : Determines the kind of data output [Integer values]
+%         '-1': Retrieves data along the magnetic field aligned beam
+%          '0': [Default mode] Retrieves data averaged across the total number 
+%               of beams 
+%    '1' or &gt;1: Assumes the number as the beam number along which you would 
+%               like the data to be retrieved</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% yNew    : 2D matrix [NxM*], where N is the time dimension and M* is the cropped altitude dimension
+% altNew  : The cropped altitude array</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+%  y       : 2D matrix [NxM], where N is the time dimension and is monotonically
+%             increasing; while M is the altitude dimension
+%  alt      : Altitude array
+%  minAlt : Lower limit of cropped altitude dimension 
+%  maxAlt : Upper limit of cropped altitude dimension</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% pfisrGD         : Geodata object of PFISR
+% coordinateNo : The coordinate number to be used to estimate the numbero
+%                      of beams (usually the slant height)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% nBeams : The number of beams present in the experiment by PFISR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% matrix - Any real valued matrix
+% newRowSize - Row size of the new matrix
+% newColSize - Col size of the new matrix</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% newMatrix - The new matrix interpolated with the new row and column size</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cumuEnergyFlux : cumulative energy flux [eV m-2 sr-1 s-1] [nExnT]
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% energyFlux : differential energy flux [eV m-2 sr-1 s-1 ev-1] [nExnT]
+% energyBin  : energy bin values [eV]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% energyFlux : NxM matrix [eV cm^-2 sr^-1 s^-1 eV^-1] or [eV m^-2 sr^-1 s^-1 eV^-1]
+% time       : 1xM matrix [s]
+% energyBins : Nx1 energy [eV]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% pfisrGD      - Data interpolated to beams parallel to mag. field line and
+%                    coordinates in xEast, yNorth, zUp
+% magcoords  - [xEast, yNorth, zUp] 
+% atTime       - Beginning and end time of the data in matlab time units
+% atAltitude   - The altitude where the coordinates of beams parallel to magnetic field
+%                   lines coincide with the actual beam coordinates </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% pfisrGD      - coordinates of pfisrGD data should be in aer coordinates
+% thisTimeStr  - Time string where you wish the data to be interpolated
+% thisAltitude - Altitude where the beam coordinates will be </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% B - Interpolated altitude vs. time matrix, along the altitude directon
+%     with nans removed [nh x nT]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+A - Input altitude vs. time matrix [nh x nT]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% lat      - latitude in deg [nCoordinates x 1]
+% lon      - longtude in deg [nCoordinates x 1]
+% altitude - in km [nCoordinates x 1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% magcoords - [nCoordinates x nDimenson]
+%     (:,1) - East  [km]
+%     (:,2) - North [km]
+%     (:,3) - Up    [km]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% ax1 - map axes
+% h   - pcolor handle of color plot of the optical data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% dataNew - 2-D optical data from DASC in geodetic coordinates [nCoordinates]
+% time    - Matlab time of the particular DASC image [nCoordinates]
+% lat     - latitude coordinates [nCoordinates]
+% lon     - longitude coordinates [nCoordinates]
+% imageSize - the total pixel size of the output image e.g. 1024 
+% latLim    - latitude limits e.g. [61 65]
+% lonLim    - longitude limits e.g. [141.5 144.5]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% Ne    : Electron density [m^-3]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% q     : Production rate [m^-3 s^-1]
+% alt   : height [length(height) x 1] [km]
+% time  : time  [1 x length(time)] [s]
+% alpha : User defined effective recombination coefficients 
+%         per altitude point [m^3 s^-1]
+%         Default: Vickerey et al., 1982</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% rotatedArray - rotated array in degrees [nArray]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% array - any array consisting of angles in degrees [nArray]
+% alpha - the angle through which the elements of the array are to be rotated [in deg]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%  yNew    : Cropped 2D matrix [NxM], where M* is the cropped time dimension
+%  timeNew : Cropped time Array </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%  y       : 2D matrix [NxM], where M is the time dimension
+%  time    : Time Array 
+%  timeMin :  Initial crop time in matlab time units
+%  timeMax :  Final crop time in matlab time units</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="146">
   <si>
     <t>Folder</t>
   </si>
@@ -812,12 +1948,291 @@
   <si>
     <t xml:space="preserve"> error_in_q, q, qTime </t>
   </si>
+  <si>
+    <t>get_inverted_flux</t>
+  </si>
+  <si>
+    <t>q, time, alt, energyBin, A, guessFlux, DateNumBeg, DateNumEnd</t>
+  </si>
+  <si>
+    <t>data                     -&gt; flux
+-&gt; energy flux, -&gt; chi2, 
+-&gt;qInverted, -&gt;maxIter, 
+-&gt; energyBin, -&gt; time, 
+-&gt; alt, -&gt;A, -&gt;qInput</t>
+  </si>
+  <si>
+    <t>Estimate energy spectra by inverting q(z)</t>
+  </si>
+  <si>
+    <t>get_pitch_angle_distribution</t>
+  </si>
+  <si>
+    <t>differentialDirectionalNumFlux_equator, pitchAngle, L, latitude</t>
+  </si>
+  <si>
+    <t>differentialDirectionalNumFlux_latitude,
+    pitchAngleAtLatitude, invariantLatitude</t>
+  </si>
+  <si>
+    <t>Calculates the pitch angle distribution from input equatorial pitch angle distribution at any latitude on a particular field line</t>
+  </si>
+  <si>
+    <t>get_production_rate</t>
+  </si>
+  <si>
+    <t>Ne, alt, time, mode, alpha</t>
+  </si>
+  <si>
+    <t>q, qTime, alpha</t>
+  </si>
+  <si>
+    <t>Estimates the production rate from measured electron density, assuming Vickery et al. model of ion chemistry</t>
+  </si>
+  <si>
+    <t>Calculates time average flux given the time limits</t>
+  </si>
+  <si>
+    <t>get_time_avg_time_series_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data, time, timeMin, timeMax </t>
+  </si>
+  <si>
+    <t>timeAvgData</t>
+  </si>
+  <si>
+    <t>kappa_E</t>
+  </si>
+  <si>
+    <t>energyBin, meanEnergy, T, kappa</t>
+  </si>
+  <si>
+    <t>noParticles</t>
+  </si>
+  <si>
+    <t>Normalized Energy distribution function (noParticles) for particles with mean energy  E0,T, and kappa value kappa.</t>
+  </si>
+  <si>
+    <t>kappa_j</t>
+  </si>
+  <si>
+    <t>x, energyBin</t>
+  </si>
+  <si>
+    <t>numberFlux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized flux (j(energyBin)) for particles with bulk energy (/velocity) meanEnergy,T,plasmaDensity, and kappa value k.
+</t>
+  </si>
+  <si>
+    <t>plot_2D_energy_slice</t>
+  </si>
+  <si>
+    <t>data, magcoords, energyBin, nBeams, timeNo, altitude, energy, setMapOn</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>Plot 2D differential energy flux slices from 4-D PFISR data sets</t>
+  </si>
+  <si>
+    <t>Should be in plotting</t>
+  </si>
+  <si>
+    <t>read_all_sky_fits</t>
+  </si>
+  <si>
+    <t>Not sure about this function</t>
+  </si>
+  <si>
+    <t>Read from .FITS file from the Digital All Sky Camera?</t>
+  </si>
+  <si>
+    <t>beamNo, latitude, longitude, altitudeGrid</t>
+  </si>
+  <si>
+    <t>read_pfisr_beam_coordinates</t>
+  </si>
+  <si>
+    <t>fileNameStr, msrParameter, altitudeGrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculates the coordinates of measurement parameters varying with altitude along different beams of PFISR (Poker Flat Incoherent Radar) system. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculates the value of the parmater specified in 'msrParameter' along altitude from measurements along the different beams of PFISR (Poker Flat Incoherent Radar) system. </t>
+  </si>
+  <si>
+    <t>read_pfisr_variable</t>
+  </si>
+  <si>
+    <t>fileNameStr, msrParameter, mode, altitudeGrid</t>
+  </si>
+  <si>
+    <t>msrParValue, altitudeGrid, time</t>
+  </si>
+  <si>
+    <t>Convert</t>
+  </si>
+  <si>
+    <t>altitude_crop</t>
+  </si>
+  <si>
+    <t>yNew, altNew</t>
+  </si>
+  <si>
+    <t>y, alt, minAlt, maxAlt</t>
+  </si>
+  <si>
+    <t>Crop Matrix Y with N time values and M altitude values to M* altitude values</t>
+  </si>
+  <si>
+    <t>calculate_nBeams</t>
+  </si>
+  <si>
+    <t>pfisrGD, coordinateNo</t>
+  </si>
+  <si>
+    <t>nBeams</t>
+  </si>
+  <si>
+    <t>Calculate the number of beams in PFISR experiment using the range, or slant_height coordinate - which is same for all beams</t>
+  </si>
+  <si>
+    <t>change_matrix_size</t>
+  </si>
+  <si>
+    <t>matrix, newRowSize, newColSize</t>
+  </si>
+  <si>
+    <t>newMatrix</t>
+  </si>
+  <si>
+    <t>Changes the size of the matrix by interpolating within</t>
+  </si>
+  <si>
+    <t>diff_to_cumu_flux</t>
+  </si>
+  <si>
+    <t>energyFlux, energyBin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cumuEnergyFlux </t>
+  </si>
+  <si>
+    <t>Converts differential energy flux into cumulative energy flux</t>
+  </si>
+  <si>
+    <t>Converting differential energy flux to differential number flux</t>
+  </si>
+  <si>
+    <t>energy_to_num</t>
+  </si>
+  <si>
+    <t>energyFlux, time, energyBin</t>
+  </si>
+  <si>
+    <t>geodata_magnetic_field_interpolation</t>
+  </si>
+  <si>
+    <t>pfisrGD, minTimeStr, maxTimeStr, thisAltitude, magBeamNo</t>
+  </si>
+  <si>
+    <t>pfisrGD, magcoords, atTime, atAltitude</t>
+  </si>
+  <si>
+    <t>Interpolate geodata beam coordinates along magnetic field direction</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>interp_nans</t>
+  </si>
+  <si>
+    <t>Removes nan by interpolating along altitude</t>
+  </si>
+  <si>
+    <t>magcoords_ned2geodetic</t>
+  </si>
+  <si>
+    <t>magcoords</t>
+  </si>
+  <si>
+    <t>lat,lon,altitude</t>
+  </si>
+  <si>
+    <t>Convert magnetic field aligned ned coordinates to geodetic at PFISR</t>
+  </si>
+  <si>
+    <t>plot_DASC_geodetic</t>
+  </si>
+  <si>
+    <t>dataNew, time, lat, lon, imageSize, latLim, lonLim</t>
+  </si>
+  <si>
+    <t>ax1,h</t>
+  </si>
+  <si>
+    <t>Plot DASC optical image in geodetic coordinates on a map</t>
+  </si>
+  <si>
+    <t>q_to_Ne</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>q, alt, time, alpha</t>
+  </si>
+  <si>
+    <t>Estimates electron density from given production rates using static recombination coefficients</t>
+  </si>
+  <si>
+    <t>rotate_array</t>
+  </si>
+  <si>
+    <t>array, alpha</t>
+  </si>
+  <si>
+    <t>rotatedArray</t>
+  </si>
+  <si>
+    <t>Rotate the array clockwise w.r.t data (and counter-clockwise w.r.t to previous configuration)</t>
+  </si>
+  <si>
+    <t>time_crop</t>
+  </si>
+  <si>
+    <t>yNew,timeNew</t>
+  </si>
+  <si>
+    <t>y,time,timeMin, timeMax</t>
+  </si>
+  <si>
+    <t>Crop a 2D matrix NxM, with time dimension M to a new time dimension M*&lt;M</t>
+  </si>
+  <si>
+    <t>unix_to_matlab_time</t>
+  </si>
+  <si>
+    <t>Converts unix time to matlab time</t>
+  </si>
+  <si>
+    <t>mTime</t>
+  </si>
+  <si>
+    <t>uTime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +2291,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -897,7 +2332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -934,6 +2369,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,16 +2653,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="19.08984375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" style="9" customWidth="1"/>
     <col min="3" max="3" width="22" style="8" customWidth="1"/>
     <col min="4" max="4" width="26.08984375" style="10" customWidth="1"/>
     <col min="5" max="5" width="38.7265625" style="5" customWidth="1"/>
@@ -1458,9 +2896,340 @@
         <v>42759</v>
       </c>
     </row>
+    <row r="14" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B28" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added root_path.m, and edited comments of many files
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="17930" windowHeight="10040"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="17930" windowHeight="10040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1772,12 +1772,541 @@
         </r>
       </text>
     </comment>
+    <comment ref="D37" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% TTick       : Time Tick values which ought to be labelled in MATLAB units
+% TTickLim    : The min and max value of time axis in MATLAB units
+% newAxisTime : [1xN] Time array of the new axis tick values
+% newAxisValue: [1xN] Array of new axis values (Example: s/c position)
+% newAxisLabel: The label of the new axis
+% axisNo      : Integer values specifying the number of the axes. This
+%               integer will determine the distance of the labels from 
+%               the axis line</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% isThereNAN : A boolean variable, True =&gt; there is nan values in the
+%                   array, and False =&gt; there is no nan values in the array
+% totalNAN   : The total number of NAN values</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% thisArray : An array or a matrix</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% local       - Structure containg details of the local peaks in the energy spectra 
+%      -&gt;pk   - Energy flux value of the peak
+%      -&gt;locs - Location of the peak / energy value
+%      -&gt;pkno - Number of the peak
+% thdEflux    - An array of themis eflux values at thisTime
+% thdeBin     - An array of themis energy bin values at thisTime
+% pfisrEflux    - An array of PFISR eflux values at thisTime
+% pfisreBin     - An array of PFISR energy bin values at thisTime</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D39" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% thisTimeStr - String of the time instant of interest e.g. 26 Mar 2008
+%               11:00 am
+% thd_time    - Time array in matlab units for THEMIS data [nTx1}
+% thd_eflux   - 2-D energy flux matrix [nExnT]
+% thd_eBin    - Energy bin array [nEx1]
+% pfisr_time  - Time array in matlab units for PFISR data [nTx1]
+% pfisr_eflux - 2-D energy flux matrix [nExnT]
+% pfisr_eBin  - Energy bin array [nEx1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% TTick     : Matlab time values where a axis tick ought to be displayed
+% DateNumBeg: Lower time limit of the axes
+% DateNumEnd: Upper time limit of the axes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% time     : Time array in matlab units [1xN]
+% timeTick : Time tick interval in hr: example - 0.5 will produce half hour
+%            intervals
+% timeMinStr: The beginning time value [in string Example: 26 Mar 2008
+%             11:00]
+% timeMaxStr: The end time value [in string]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D43" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% time          : 1xN - A time array [matlab units]
+% setLabel      : true or false, if true there will be  tick marks, and labels
+%                 if false there will be only tick marks
+% timeTick      : Value of time interval between tick marks [Hr]
+% timeMinStr    : Minimum value of time [String] Ex: '26 Mar 2008 11:00'
+% timeMaxStr    : Maximum value of time [String] Ex: '26 Mar 2008 11:00'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% p         : plot handle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D44" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%  time  : 1xN - A time array [matlab units]
+%  yAxis  : Mx1 - Values of the parameter on vertical axis (y-axis)
+%                 Example: Energy bin [eV]
+%  zValue  : MxN - A matrix specifying zValue along time and y-axis
+%                 Example: Energy flux [eV/ cm^2 sec sr eV]
+%  timeTime : Value of time at which to plot [String]
+%  mode     : Uses a set of pre-determined plot options
+%       '-1': Assumes loglog(yAxis,zValueThisTime) with no labels [Default]
+%        '0': Assumes semilogx(zValueThisTime,yAxis) with no labels 
+%   '1': Assumes one is plotting Electron Density
+%        '2': Assumes one is plotting Production rates
+%        '3': Assumes one is plotting Differential Energy Flux</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% h         : pcolor handle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%  time  : 1xN - A time array [matlab units]
+%  yAxis  : Mx1 - Values of the parameter on vertical axis (y-axis)
+%                 Example: Energy bin [eV]
+%  zValue  : MxN - A matrix specifying zValues along time and y-axis
+%                 Example: Energy flux [eV/ cm^2 sec sr eV]
+%  timeTick : Value of time interval between tick marks [Hr]
+%  mode     : Uses a set of pre-determined plot options
+%        '1': Assumes one is plotting Electron Density
+%        '2': Assumes one is plotting Production rates
+%        '3': Assumes one is plotting Differential Energy Flux
+% timeMin   : Minimum value of time [String] Ex: '26 Mar 2008 11:00'
+% timeMax   : Maximum value of time [String] Ex: '26 Mar 2008 11:00'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% dataNew - 2-D optical data from DASC in geodetic coordinates [nCoordinates]
+% az     - Azimuth coordinates [nCoordinates]
+% el     - Elevation coordinates [nCoordinates]
+% imageSize - the total pixel size of the output image e.g. 1024 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% h          - pcolor plot handle of plot_2D_time_series</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% data      - 2-D optical data from DASC in geodetic coordinates [nCoordinates]
+% aercoords - Azimuth, elevation, and range coordinates [nCoordinates x 3]
+% energyBin - Array with values of energy bin
+% nBeams    - Total number of beams
+% timeMinStr - Lower limit of time in string
+% timeMaxStr - Upper limit of time in string
+% altitude   - The altitude at which the keogram is projected 
+% energy     - The energy to be plotted</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% az        - Array of azimuth values to plot grid lines
+% el        - Array of elevation values to plot grid lines
+% colorStr  - Color of the grid lines e.g. 'r'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% dataChoice - Array of numbers - each number associated with a data set 
+%              to be plotted in order</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% figureHandle
+% vert - Vertical page size in mm (Default Letter Size)
+% horz - Horizontal page size in mm (Default Letter Size)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B52" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% rootPathStr - A string containg git directory path in the present computer</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="198">
   <si>
     <t>Folder</t>
   </si>
@@ -2227,12 +2756,168 @@
   <si>
     <t>uTime</t>
   </si>
+  <si>
+    <t>Plotting &amp; Misc</t>
+  </si>
+  <si>
+    <t>Add additional XTickLabels below the existing time axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TTick, TTickLim, newAxisTime, newAxisValue, newAxisLabel, axisNo</t>
+  </si>
+  <si>
+    <t>add_horizontal_axes</t>
+  </si>
+  <si>
+    <t>Check if there is any nan values in the given array</t>
+  </si>
+  <si>
+    <t>thisArray</t>
+  </si>
+  <si>
+    <t>check_nan</t>
+  </si>
+  <si>
+    <t>isThereNAN, totalNAN</t>
+  </si>
+  <si>
+    <t>find_peaks</t>
+  </si>
+  <si>
+    <t>thisTimeStr, thd_time, thd_eflux, thd_eBin, pfisr_time, pfisr_eflux, pfisr_eBin</t>
+  </si>
+  <si>
+    <t>local, thdEflux, thdeBin, pfisrEflux, pfisreBin</t>
+  </si>
+  <si>
+    <t>Identify peaks in the energy spectra of THEMIS and PFISR</t>
+  </si>
+  <si>
+    <t>get_axes_time_tick_values</t>
+  </si>
+  <si>
+    <t>time, timeTick, timeMinStr, timeMaxStr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTick, DateNumBeg, DateNumEnd </t>
+  </si>
+  <si>
+    <t>Calculates the time tick values in matlab units</t>
+  </si>
+  <si>
+    <t>include_new_colormaps</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>The function initializes a few colormaps, given the path of the color maps</t>
+  </si>
+  <si>
+    <t>initialize_geodata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time, setLabel, timeTick, timeMinStr, timeMaxStr </t>
+  </si>
+  <si>
+    <t>label_time_axis</t>
+  </si>
+  <si>
+    <t>Sets the time axis (x-axis) time-tick locations and labels</t>
+  </si>
+  <si>
+    <t>time, yAxis, zValue, thisTime, mode</t>
+  </si>
+  <si>
+    <t>plot_1D_time_slice</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Plots the 1-D energy flux using an input data structure</t>
+  </si>
+  <si>
+    <t>data, aercoords, energyBin, nBeams, timeNo, altitude, energy, setMapOn</t>
+  </si>
+  <si>
+    <t>plot_2D_energy_slice_aer</t>
+  </si>
+  <si>
+    <t>Plot 2D energy flux map at a particular time, energy and projected at an altitude</t>
+  </si>
+  <si>
+    <t>plot_2D_time_series</t>
+  </si>
+  <si>
+    <t>time, yAxis, zValue, timeTick, mode, timeMinStr, timeMaxStr</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Plots 2D time series data</t>
+  </si>
+  <si>
+    <t>plot_DASC_aer</t>
+  </si>
+  <si>
+    <t>Plots the All Sky Image in az, el, range coordinates</t>
+  </si>
+  <si>
+    <t>dataNew, az, el, imageSize</t>
+  </si>
+  <si>
+    <t>data, aercoords, energyBin, nBeams, timeMinStr, timeMaxStr, altitude, energy</t>
+  </si>
+  <si>
+    <t>plot_energyflux_keogram</t>
+  </si>
+  <si>
+    <t>plot_grid_aer</t>
+  </si>
+  <si>
+    <t>az, el, colorStr</t>
+  </si>
+  <si>
+    <t>Plot 2-D keogram of enegry flux at particular energy</t>
+  </si>
+  <si>
+    <t>Plots grid lines in polar plot at specified azimuth and elevation</t>
+  </si>
+  <si>
+    <t>plot_preset_data_panels</t>
+  </si>
+  <si>
+    <t>dataChoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plots data from the choices in panel form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">figureHandle, vert, horz </t>
+  </si>
+  <si>
+    <t>resize_figure</t>
+  </si>
+  <si>
+    <t>Resizes figure into a standard paper size</t>
+  </si>
+  <si>
+    <t>Generates the root git-hub path based on the computer</t>
+  </si>
+  <si>
+    <t>rootPathStr</t>
+  </si>
+  <si>
+    <t>root_path</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2311,6 +2996,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2320,7 +3011,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2328,20 +3019,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2350,9 +3146,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2370,14 +3163,229 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2388,6 +3396,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E52" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E52"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Folder" dataDxfId="4"/>
+    <tableColumn id="2" name="Output" dataDxfId="3"/>
+    <tableColumn id="3" name="Function Name" dataDxfId="2"/>
+    <tableColumn id="4" name="Input" dataDxfId="1"/>
+    <tableColumn id="5" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2653,59 +3675,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="20.26953125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="22" style="8" customWidth="1"/>
-    <col min="4" max="4" width="26.08984375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="38.7265625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="8">
         <v>42773</v>
       </c>
       <c r="G2" t="s">
@@ -2713,284 +3735,303 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="8">
         <v>42725</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>42634</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>42634</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>42725</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>42634</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>42760</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>42760</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>42634</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>42638</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>42635</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>42759</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="17" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="17" t="s">
         <v>82</v>
       </c>
       <c r="G20" t="s">
@@ -2998,16 +4039,17 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="17" t="s">
         <v>86</v>
       </c>
       <c r="G21" t="s">
@@ -3015,221 +4057,460 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="A22" s="16"/>
+      <c r="B22" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="16"/>
+      <c r="B28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="17" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="17" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="17" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="17" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B32" s="9" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="9" t="s">
+    <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="16"/>
+      <c r="B33" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="9" t="s">
+    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="16"/>
+      <c r="B34" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="9" t="s">
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="16"/>
+      <c r="B35" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="9" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="16"/>
+      <c r="B36" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="17" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="16"/>
+      <c r="B38" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="16"/>
+      <c r="B39" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="16"/>
+      <c r="B40" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="16"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="16"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="16"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="16"/>
+      <c r="B44" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="16"/>
+      <c r="B45" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="16"/>
+      <c r="B46" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="16"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="16"/>
+      <c r="B48" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="16"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="16"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="16"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="22"/>
+      <c r="B52" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" s="25"/>
+      <c r="E52" s="26" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Conductivity & Wrapping up Paper 1
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="17930" windowHeight="10040"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="17930" windowHeight="10040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -710,6 +710,59 @@
         </r>
       </text>
     </comment>
+    <comment ref="B17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% Output:
+%  timeNo: The index of the time array that points 
+%             to the time specified by thisTime </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% Input
+%  time     : 1-D time Array 
+%  thisTime : String identifying the time to be found 
+%             from the array time '26 Mar 2008 11:00'</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B18" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1720,7 +1773,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B35" authorId="0" shapeId="0">
+    <comment ref="B36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1746,7 +1799,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="0" shapeId="0">
+    <comment ref="D36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1770,7 +1823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B38" authorId="0" shapeId="0">
+    <comment ref="B39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1794,7 +1847,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D39" authorId="0" shapeId="0">
+    <comment ref="D40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1821,7 +1874,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D40" authorId="0" shapeId="0">
+    <comment ref="D41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1852,7 +1905,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="0" shapeId="0">
+    <comment ref="B42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1883,7 +1936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0">
+    <comment ref="D42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1914,7 +1967,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0" shapeId="0">
+    <comment ref="B43" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1940,7 +1993,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="0" shapeId="0">
+    <comment ref="D43" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1969,7 +2022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D43" authorId="0" shapeId="0">
+    <comment ref="D44" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1998,7 +2051,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0" shapeId="0">
+    <comment ref="B45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2022,7 +2075,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D44" authorId="0" shapeId="0">
+    <comment ref="D45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2057,7 +2110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0">
+    <comment ref="B47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2081,7 +2134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D46" authorId="0" shapeId="0">
+    <comment ref="D47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2122,7 +2175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0" shapeId="0">
+    <comment ref="B48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2146,7 +2199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D47" authorId="0" shapeId="0">
+    <comment ref="D48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2181,7 +2234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="0" shapeId="0">
+    <comment ref="D49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2208,7 +2261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0" shapeId="0">
+    <comment ref="B50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2233,7 +2286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D49" authorId="0" shapeId="0">
+    <comment ref="D50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2263,7 +2316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0" shapeId="0">
+    <comment ref="B51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2287,7 +2340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="0" shapeId="0">
+    <comment ref="D51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2318,7 +2371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2344,7 +2397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="0" shapeId="0">
+    <comment ref="D53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2374,7 +2427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="202">
   <si>
     <t>Folder</t>
   </si>
@@ -2979,12 +3032,24 @@
   <si>
     <t>Converting differential number flux to differential energy flux</t>
   </si>
+  <si>
+    <t>get_energy_distribution_moment</t>
+  </si>
+  <si>
+    <t>flux,energyBin</t>
+  </si>
+  <si>
+    <t>mean, median</t>
+  </si>
+  <si>
+    <t>Calculates the mean and median of an input energy distribution</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3060,6 +3125,26 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3221,10 +3306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3319,29 +3405,27 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3544,6 +3628,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
@@ -3558,12 +3658,14 @@
         <right style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -3602,18 +3704,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F52" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:F52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F53" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F53"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Folder" dataDxfId="6"/>
-    <tableColumn id="2" name="Output" dataDxfId="5"/>
-    <tableColumn id="3" name="Function Name" dataDxfId="4"/>
-    <tableColumn id="4" name="Input" dataDxfId="3"/>
-    <tableColumn id="5" name="Description" dataDxfId="2"/>
-    <tableColumn id="6" name="Last Updated" dataDxfId="1"/>
+    <tableColumn id="1" name="Folder" dataDxfId="5"/>
+    <tableColumn id="2" name="Output" dataDxfId="4"/>
+    <tableColumn id="3" name="Function Name" dataDxfId="3"/>
+    <tableColumn id="4" name="Input" dataDxfId="2"/>
+    <tableColumn id="5" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" name="Last Updated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3882,17 +3984,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="20.26953125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" style="4" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
     <col min="5" max="5" width="38.7265625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.453125" style="7" bestFit="1" customWidth="1"/>
@@ -4252,7 +4354,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>180</v>
       </c>
@@ -4272,7 +4374,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>180</v>
       </c>
@@ -4312,7 +4414,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>180</v>
       </c>
@@ -4472,7 +4574,7 @@
         <v>42657</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>180</v>
       </c>
@@ -4559,7 +4661,7 @@
       <c r="B34" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="16" t="s">
@@ -4573,142 +4675,140 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>130</v>
+      <c r="A35" s="22"/>
+      <c r="B35" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>199</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" s="18">
-        <v>42635</v>
+        <v>201</v>
+      </c>
+      <c r="F35" s="36">
+        <v>42927</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="24" t="s">
-        <v>141</v>
+      <c r="B36" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="19"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+      <c r="F36" s="18">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B37" s="14"/>
-      <c r="C37" s="15" t="s">
-        <v>144</v>
+      <c r="C37" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="F37" s="19"/>
     </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="B38" s="14"/>
       <c r="C38" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F38" s="18">
-        <v>42776</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="14"/>
+      <c r="B39" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="C39" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>170</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D39" s="16"/>
       <c r="E39" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F39" s="19"/>
-    </row>
-    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="25" t="s">
-        <v>185</v>
+        <v>173</v>
+      </c>
+      <c r="F39" s="18">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="15" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F40" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="F40" s="19"/>
+    </row>
+    <row r="41" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B41" s="14" t="s">
-        <v>135</v>
-      </c>
+      <c r="B41" s="14"/>
       <c r="C41" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F41" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F42" s="18">
         <v>42759</v>
@@ -4718,58 +4818,58 @@
       <c r="A43" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B43" s="14"/>
+      <c r="B43" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="C43" s="15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F43" s="18">
-        <v>42642</v>
+        <v>42759</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="14" t="s">
-        <v>150</v>
-      </c>
+      <c r="B44" s="14"/>
       <c r="C44" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F44" s="18">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42642</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="F45" s="18">
-        <v>42759</v>
+        <v>42639</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -4780,13 +4880,13 @@
         <v>72</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F46" s="18">
         <v>42759</v>
@@ -4797,112 +4897,132 @@
         <v>185</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>154</v>
+        <v>72</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="F47" s="18">
-        <v>42658</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B48" s="14"/>
+      <c r="B48" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C48" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F48" s="18">
-        <v>42759</v>
+        <v>42658</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="B49" s="14"/>
       <c r="C49" s="15" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="F49" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="F50" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B51" s="14"/>
+      <c r="B51" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C51" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F51" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="26" t="s">
+    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="28" t="s">
+      <c r="B52" s="14"/>
+      <c r="C52" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D53" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="E53" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="F52" s="31">
+      <c r="F53" s="31">
         <v>42759</v>
       </c>
     </row>
@@ -4913,11 +5033,14 @@
   <conditionalFormatting sqref="C11">
     <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C34" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commented and added altitude range
Added function input altRange that allows one to integrate over a specific altitude range, instead of the default full altitude range.
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nithin\Documents\GitHub\energy-height-conversion\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithin\Documents\GitHub\energy-height-conversion\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="17930" windowHeight="10040"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="17928" windowHeight="10044"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nithin Sivadas</author>
+    <author>nithin</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0">
@@ -607,7 +608,72 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="0" shapeId="0">
+    <comment ref="B15" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% integratedData - sigma_H [nBeams x nT]
+%                  sigma_P [nBeams x nT]
+%                  lat     [nBeams x 1]
+%                  lon     [nBeams x 1]
+%                  projectionAltitude [1]
+%                  time   [nT x 1]
+%                  ratio  [nBeams x nT] : ratio of Hall to Pedersen conductance
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% data      - sigma_P_B [(nBeams x nh) x nT]
+%             calculated along mangetic field aligned nBeams
+%           - sigma_H_B [(nBeams x nh) x nT]
+%             calculated along magneticfield aligned beams
+%           - time [nTx1]
+%           - conductanceCoordsB [(nBeams x nh) x 3] (lat,lon,alt)
+%             calculated along magneticfield aligned beams
+% nBeams    - total number of radar beams
+% projectionAltitude - Altitude [km] at which the map ought to be projected
+% altRange  - [minAlt maxAlt] the range of altitude to be used for integration
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -633,7 +699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="0" shapeId="0">
+    <comment ref="E16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -658,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -685,7 +751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -710,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0">
+    <comment ref="B18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -736,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -763,7 +829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment ref="B19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -805,7 +871,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -837,7 +903,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0">
+    <comment ref="D20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -862,7 +928,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -888,7 +954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -912,7 +978,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -941,7 +1007,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0">
+    <comment ref="D22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -966,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="0" shapeId="0">
+    <comment ref="E22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -993,7 +1059,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1017,7 +1083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1049,7 +1115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="0" shapeId="0">
+    <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1075,7 +1141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1106,7 +1172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment ref="B25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1139,7 +1205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D24" authorId="0" shapeId="0">
+    <comment ref="D25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1168,7 +1234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E24" authorId="0" shapeId="0">
+    <comment ref="E25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1193,7 +1259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0">
+    <comment ref="B26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1217,7 +1283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0" shapeId="0">
+    <comment ref="D26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1244,7 +1310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1268,7 +1334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="0" shapeId="0">
+    <comment ref="D27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1297,7 +1363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0">
+    <comment ref="B28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1328,7 +1394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1380,7 +1446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1435,7 +1501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0">
+    <comment ref="D30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1471,7 +1537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
+    <comment ref="B31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1501,7 +1567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1539,7 +1605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0" shapeId="0">
+    <comment ref="B32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1567,7 +1633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="0" shapeId="0">
+    <comment ref="D32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1609,7 +1675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0">
+    <comment ref="B33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1636,7 +1702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="0" shapeId="0">
+    <comment ref="D33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1663,7 +1729,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1690,7 +1756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0" shapeId="0">
+    <comment ref="D34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1721,7 +1787,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0" shapeId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1746,7 +1812,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0" shapeId="0">
+    <comment ref="D35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1773,7 +1839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0" shapeId="0">
+    <comment ref="B37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1799,7 +1865,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="0" shapeId="0">
+    <comment ref="D37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1823,7 +1889,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0">
+    <comment ref="B40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1847,7 +1913,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D40" authorId="0" shapeId="0">
+    <comment ref="D41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1874,7 +1940,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0">
+    <comment ref="D42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1905,7 +1971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0" shapeId="0">
+    <comment ref="B43" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1936,7 +2002,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="0" shapeId="0">
+    <comment ref="D43" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1967,7 +2033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0" shapeId="0">
+    <comment ref="B44" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1993,7 +2059,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D43" authorId="0" shapeId="0">
+    <comment ref="D44" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2022,7 +2088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D44" authorId="0" shapeId="0">
+    <comment ref="D45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2051,7 +2117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="0" shapeId="0">
+    <comment ref="B46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2075,7 +2141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D45" authorId="0" shapeId="0">
+    <comment ref="D46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2110,7 +2176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0" shapeId="0">
+    <comment ref="B48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2134,7 +2200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D47" authorId="0" shapeId="0">
+    <comment ref="D48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2175,7 +2241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0" shapeId="0">
+    <comment ref="B49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2199,7 +2265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="0" shapeId="0">
+    <comment ref="D49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2234,7 +2300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D49" authorId="0" shapeId="0">
+    <comment ref="D50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2261,7 +2327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0" shapeId="0">
+    <comment ref="B51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2286,7 +2352,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="0" shapeId="0">
+    <comment ref="D51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2316,7 +2382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B51" authorId="0" shapeId="0">
+    <comment ref="B52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2340,7 +2406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2371,7 +2437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="0" shapeId="0">
+    <comment ref="D53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2397,7 +2463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="0" shapeId="0">
+    <comment ref="D54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2427,7 +2493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="206">
   <si>
     <t>Folder</t>
   </si>
@@ -3043,6 +3109,18 @@
   </si>
   <si>
     <t>Calculates the mean and median of an input energy distribution</t>
+  </si>
+  <si>
+    <t>num_to_energy</t>
+  </si>
+  <si>
+    <t>integratedData</t>
+  </si>
+  <si>
+    <t>integrate_conductivity</t>
+  </si>
+  <si>
+    <t>data, nBeams, projectionAltitude, altRange</t>
   </si>
 </sst>
 </file>
@@ -3310,7 +3388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3420,12 +3498,35 @@
     <xf numFmtId="14" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3668,26 +3769,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0"/>
@@ -3704,18 +3785,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F53" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:F54"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Folder" dataDxfId="5"/>
-    <tableColumn id="2" name="Output" dataDxfId="4"/>
-    <tableColumn id="3" name="Function Name" dataDxfId="3"/>
-    <tableColumn id="4" name="Input" dataDxfId="2"/>
-    <tableColumn id="5" name="Description" dataDxfId="1"/>
-    <tableColumn id="6" name="Last Updated" dataDxfId="0"/>
+    <tableColumn id="1" name="Folder" dataDxfId="7"/>
+    <tableColumn id="2" name="Output" dataDxfId="6"/>
+    <tableColumn id="3" name="Function Name" dataDxfId="5"/>
+    <tableColumn id="4" name="Input" dataDxfId="4"/>
+    <tableColumn id="5" name="Description" dataDxfId="3"/>
+    <tableColumn id="6" name="Last Updated" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3984,23 +4065,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="20.26953125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="20.21875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="38.7265625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4020,7 +4101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>79</v>
       </c>
@@ -4040,7 +4121,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -4058,7 +4139,7 @@
       </c>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>79</v>
       </c>
@@ -4078,7 +4159,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>79</v>
       </c>
@@ -4098,7 +4179,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>79</v>
       </c>
@@ -4118,7 +4199,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -4138,7 +4219,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>79</v>
       </c>
@@ -4158,7 +4239,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>79</v>
       </c>
@@ -4178,7 +4259,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>79</v>
       </c>
@@ -4198,13 +4279,13 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="14" t="s">
         <v>195</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>94</v>
+        <v>202</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>196</v>
@@ -4216,7 +4297,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>79</v>
       </c>
@@ -4236,7 +4317,7 @@
         <v>42635</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>79</v>
       </c>
@@ -4256,7 +4337,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>79</v>
       </c>
@@ -4276,623 +4357,619 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>179</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F16" s="18">
-        <v>42725</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>179</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="18">
+        <v>42725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F18" s="18">
         <v>42634</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="18">
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>31</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D19" s="16"/>
       <c r="E19" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F19" s="18">
         <v>42760</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F20" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42760</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F21" s="18">
-        <v>42638</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F22" s="18">
-        <v>42635</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F24" s="18">
-        <v>42638</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>186</v>
+        <v>50</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F25" s="18">
         <v>42638</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="F26" s="18">
         <v>42638</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="F27" s="18">
-        <v>42773</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42638</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="F28" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>42773</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F29" s="18">
-        <v>42657</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="F30" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>42657</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="F31" s="18">
         <v>42634</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F32" s="18">
-        <v>42774</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F33" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42774</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="18">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C35" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D35" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E35" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F35" s="18">
         <v>42639</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="22"/>
-      <c r="B35" s="33" t="s">
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="22"/>
+      <c r="B36" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C36" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D36" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E36" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F36" s="36">
         <v>42927</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="18">
-        <v>42635</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="24" t="s">
-        <v>141</v>
+      <c r="B37" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" s="19"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+      <c r="F37" s="18">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B38" s="14"/>
-      <c r="C38" s="15" t="s">
-        <v>144</v>
+      <c r="C38" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="F38" s="19"/>
     </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="B39" s="14"/>
       <c r="C39" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F39" s="18">
-        <v>42776</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="17"/>
+      <c r="F39" s="19"/>
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B40" s="14"/>
+      <c r="B40" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="C40" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>170</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D40" s="16"/>
       <c r="E40" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F40" s="19"/>
-    </row>
-    <row r="41" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="25" t="s">
-        <v>185</v>
+        <v>173</v>
+      </c>
+      <c r="F40" s="18">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="15" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F41" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="F41" s="19"/>
+    </row>
+    <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>135</v>
-      </c>
+      <c r="B42" s="14"/>
       <c r="C42" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F42" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F43" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="14"/>
+      <c r="B44" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="C44" s="15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F44" s="18">
-        <v>42642</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B45" s="14" t="s">
-        <v>150</v>
-      </c>
+      <c r="B45" s="14"/>
       <c r="C45" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F45" s="18">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42642</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="F46" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
         <v>185</v>
       </c>
@@ -4900,141 +4977,161 @@
         <v>72</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F47" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>154</v>
+        <v>72</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="F48" s="18">
-        <v>42658</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B49" s="14"/>
+      <c r="B49" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C49" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F49" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>42658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="B50" s="14"/>
       <c r="C50" s="15" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="F50" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="F51" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B52" s="14"/>
+      <c r="B52" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C52" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F52" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="26" t="s">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28" t="s">
+      <c r="B53" s="14"/>
+      <c r="C53" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F53" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D54" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="E54" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="F53" s="31">
+      <c r="F54" s="31">
         <v>42759</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C10 C12:C1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C34" r:id="rId1"/>
+    <hyperlink ref="C35" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>

</xml_diff>

<commit_message>
half way into automating processes to calculate and plot energy flux maps
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="17928" windowHeight="10044"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="17928" windowHeight="4104"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2493,7 +2493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="207">
   <si>
     <t>Folder</t>
   </si>
@@ -3121,6 +3121,9 @@
   </si>
   <si>
     <t>data, nBeams, projectionAltitude, altRange</t>
+  </si>
+  <si>
+    <t>Integrates beam-wise conductivity along altitude</t>
   </si>
 </sst>
 </file>
@@ -3509,26 +3512,6 @@
   <dxfs count="12">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3769,6 +3752,26 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0"/>
@@ -3785,18 +3788,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F54"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Folder" dataDxfId="7"/>
-    <tableColumn id="2" name="Output" dataDxfId="6"/>
-    <tableColumn id="3" name="Function Name" dataDxfId="5"/>
-    <tableColumn id="4" name="Input" dataDxfId="4"/>
-    <tableColumn id="5" name="Description" dataDxfId="3"/>
-    <tableColumn id="6" name="Last Updated" dataDxfId="2"/>
+    <tableColumn id="1" name="Folder" dataDxfId="5"/>
+    <tableColumn id="2" name="Output" dataDxfId="4"/>
+    <tableColumn id="3" name="Function Name" dataDxfId="3"/>
+    <tableColumn id="4" name="Input" dataDxfId="2"/>
+    <tableColumn id="5" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" name="Last Updated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4067,8 +4070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4370,8 +4373,12 @@
       <c r="D15" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="36"/>
+      <c r="E15" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F15" s="36">
+        <v>43102</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
@@ -5125,10 +5132,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C10 C12:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C35" r:id="rId1"/>

</xml_diff>

<commit_message>
Sample update from Windows PC
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithin\Documents\GitHub\energy-height-conversion\Tools\"/>
@@ -2493,7 +2493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="207">
   <si>
     <t>Folder</t>
   </si>
@@ -4070,8 +4070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4779,7 +4779,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
+      <c r="A36" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="B36" s="33" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
Revert "Sample update from Windows PC"
This reverts commit 415015a1391a5942aa8deb90b60f8a320f523b76.
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithin\Documents\GitHub\energy-height-conversion\Tools\"/>
@@ -2493,7 +2493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="207">
   <si>
     <t>Folder</t>
   </si>
@@ -4070,8 +4070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4779,9 +4779,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
-        <v>180</v>
-      </c>
+      <c r="A36" s="22"/>
       <c r="B36" s="33" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
Completed making sure create-magneticFieldProjections_hdf5 will work with low memory
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="17928" windowHeight="4104"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="17280" windowHeight="4104"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -744,6 +744,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+% medianIndex : The index number of the energy bin array which cuts the 
+%                     cumulative energy flux distribution in half</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 % array : A 2-D array - [Energy x Time] of normalized cimulative energy
 %         flux
 % dim   : The energy dimension - by default 1 as per above definition of
@@ -751,32 +776,241 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nithin Sivadas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-% medianIndex : The index number of the energy bin array which cuts the 
-%                     cumulative energy flux distribution in half</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment ref="B18" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% magBeamNo             - Field aligned beam number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% beamCodes             - [nPos x nBeams] Beam code for each azimuth and elevation coordinate.
+% magFieldAlignedAz     - The azimuth value of the field line from the radar center
+% magFieldAlignedElev   - The elevation value of the field line from the radar centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%   flag    "1" - conjunction
+%           "0" - no conjunction
+%   probeNames  - fieldnames of probe.(field) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%   probes.(field).GDZ           - [lat, lon, alt] of a spacecraft
+%   conjunctionCoords.GDZ     - [lat, lon, alt] of probe/ground-location with which you wish to check conjunction.
+%   conjunctionCoords.radius   - [in km] The acceptable radius of conjunction
+%   stopAlt                          - [in km] Altitude at which conjunction is to be determined
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% probes:
+% -&gt; flag : [nTxnProbes] Each element in this array corresponds to a time
+%        point and probe. If the value is +1, at that time point that
+%        particular probe is in magnetic conjunction as defined by the
+%        conjunction.radius with conjunction.probeStr. If it is 0, then
+%        there is no conjunction.
+%   -&gt; probeNames: [1xnProbes][cell] Each element corresponds to column in flag, 
+%                  and is the name of the probe that it corresponds to.  
+%   -&gt; GDZ       : [nT x 2] Lat and Lon coordinates of the probe for
+%                  the correspoinding input times
+%   -&gt; GEO       : [nT x 3] X,Y,Z- GEO cartesian coordinates of probes 
+%                  which are spacecrafts</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% time      : [nTx1] [u:matlabtime] An array of time points at which you need
+%             to estimate magnetic conjunction
+%             Default:'26 Mar 2008'
+% omniData  : Data product of process_omni_data.m Contains
+%             omniData.minutely.maginput, for estimate the magnetic field
+%             model
+% spacecraft: 
+%   -&gt; (probename).GEO: [nTx3] Time series position coordinates of a
+%                       spacecraft in GEO coordinate system. There can be
+%                       more than one probename. Example spacraft.thma,
+%                       spacecraft.thmb and so on in the same structure. 
+%   -&gt; (probename).time: [nTx1] An array of time points corresponding to
+%                        the spacecraft position data. 
+% groundstation:
+%   -&gt; GDZ            : [1x2] Latitude and Longitude of the ground station.
+%   -&gt; field          : [string] A short name of the ground station.
+%                       Example: 'pokerflat'
+% conjunction:
+%   -&gt; probeStr       : [string] Select the spacecraft or ground station
+%                       with respect to which the magnetic field
+%                       conjunction of the other probes ought to be
+%                       calculated
+%                       Example: 'pokerflat' or 'thma'
+%   -&gt; radius         : [1][km] Radius of the circle within which the
+%                       geodetic coordinates of the probes have to fall to
+%                       be considered as magnetically conjugate with
+%                       probeStr. 
+% stopAlt   : [km] The altitude at which the magnetic foot point of the
+%             spacecraft ought to be calculated. 
+%             Default: 110km
+% hemiFlag  : A flag value to specify the hemisphere of conjunction 
+%                0  - same Hemisphere as start point
+%               +1  - Northern Hemisphere
+%               -1  - Southern Hemisphere
+%                2  - opposite Hemisphere as start point
+%            Default: +1
+%
+% magFieldModel: Flat specifying which magnetic field to use. Default:11
+%                 0   = no external field 
+%                 1   = Mead &amp; Fairfield [1975] 
+%                     (uses 0?Kp?9 - Valid for rGEO?17. Re) 
+%                 2   = Tsyganenko short [1987] 
+%                     (uses 0?Kp?9 - Valid for rGEO?30. Re) 
+%                 3   = Tsyganenko long [1987] 
+%                     (uses 0?Kp?9 - Valid for rGEO?70. Re) 
+%                 4   = Tsyganenko [1989c] 
+%                     (uses 0?Kp?9 - Valid for rGEO?70. Re) 
+%                 5   = Olson &amp; Pfitzer quiet [1977] 
+%                     (default - Valid for rGEO?15. Re) 
+%                 6   = Olson &amp; Pfitzer dynamic [1988] 
+%                     (uses 5.?dens?50., 300.?velo?500., 
+%                     -100.?Dst?20. - Valid for rGEO?60. Re) 
+%                 7   = Tsyganenko [1996] 
+%                     (uses -100.?Dst (nT)?20., 0.5?Pdyn (nPa)?10., 
+%                     |ByIMF| (nT)?10., |BzIMF| (nT)?10. - Valid for rGEO?40. Re) 
+%                 8   = Ostapenko &amp; Maltsev [1997] 
+%                     (uses dst,Pdyn,BzIMF, Kp) 
+%                 9   = Tsyganenko [2001] 
+%                     (uses -50.?Dst (nT)?20., 0.5?Pdyn (nPa)?5., |ByIMF| (nT)?5., 
+%                     |BzIMF| (nT)?5., 0.?G1?10., 0.?G2?10. - Valid for xGSM?-15. Re) 
+%                 10 =Tsyganenko [2001] storm  
+%                     (uses Dst, Pdyn, ByIMF, BzIMF, G2, G3 
+%                     - there is no upper or lower limit 
+%                     for those inputs - Valid for xGSM?-15. Re) 
+%                 11 =Tsyganenko [2004] storm  
+%                     (uses Dst, Pdyn, ByIMF, BzIMF, 
+%                     W1, W2, W3, W4, W5, W6 
+%                     - there is no upper or lower limit for those inputs 
+%                     - Valid for xGSM?-15. Re) 
+%                 12 =Alexeev [2000] 
+%                     - also known as Paraboloid model - 
+%                     Submitted to ISO  (uses Dens, velo, Dst, BzIMF, AL) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -802,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0">
+    <comment ref="D21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -829,7 +1063,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -871,7 +1105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -903,7 +1137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -928,7 +1162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -954,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0">
+    <comment ref="D24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -978,7 +1212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1007,7 +1241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0">
+    <comment ref="D25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1032,7 +1266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0">
+    <comment ref="E25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1059,7 +1293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="0" shapeId="0">
+    <comment ref="B26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1083,7 +1317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1115,7 +1349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1141,7 +1375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D24" authorId="0" shapeId="0">
+    <comment ref="D27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1172,7 +1406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0">
+    <comment ref="B28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1205,7 +1439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1234,7 +1468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="0" shapeId="0">
+    <comment ref="E28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1259,7 +1493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment ref="B29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1283,7 +1517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="0" shapeId="0">
+    <comment ref="D29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1310,7 +1544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1334,7 +1568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0">
+    <comment ref="D30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1363,7 +1597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1394,7 +1628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1420,7 +1654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0">
+    <comment ref="B32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1446,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0">
+    <comment ref="D32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1470,7 +1704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
+    <comment ref="B33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1501,7 +1735,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1537,7 +1771,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0" shapeId="0">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1567,7 +1801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="0" shapeId="0">
+    <comment ref="D34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1605,7 +1839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1633,7 +1867,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="0" shapeId="0">
+    <comment ref="D35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1675,7 +1909,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0">
+    <comment ref="B36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1702,7 +1936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0" shapeId="0">
+    <comment ref="D36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1729,7 +1963,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0" shapeId="0">
+    <comment ref="B37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1756,7 +1990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0" shapeId="0">
+    <comment ref="D37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1787,7 +2021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B35" authorId="0" shapeId="0">
+    <comment ref="B38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1812,7 +2046,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="0" shapeId="0">
+    <comment ref="D38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1839,108 +2073,183 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Nithin Sivadas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-% isThereNAN : A boolean variable, True =&gt; there is nan values in the
-%                   array, and False =&gt; there is no nan values in the array
-% totalNAN   : The total number of NAN values</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Nithin Sivadas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-% thisArray : An array or a matrix</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B40" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Nithin Sivadas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-% rootPathStr - A string containg git directory path in the present computer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D41" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Nithin Sivadas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-% figureHandle
-% vert - Vertical page size in mm (Default Letter Size)
-% horz - Horizontal page size in mm (Default Letter Size)
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D42" authorId="0" shapeId="0">
+    <comment ref="B42" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% table            : Cell array with details of the experiments from amisr
+%                    webpage
+% tableHeader      : Cell array with column names</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D42" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% timeMinStr      : [String] The start time from which you want experiment
+%                   details
+%                   Default:'5 Jan 2017'
+% timeMaxStr      : [String] The start time from which you want experiment
+%                   details
+%                   Default:'5 Feb 2017'
+% InstrumentID    : [Integer] Madrigal ID number of the instrument
+%                   Default:61
+%                   This specified poker flat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%   outputArguments.sigma_P  - Pederson conductivity [S/m]
+%   outputArguments.sigma_H  - Hall conductivity [S/m]
+%   outputArguments.alt      - Altitude [km]
+%   and  a lot of other things</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D43" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+%   alt                      - Altitude array [nHx1] [km]
+%   electronDensity          - Electron denisity input [nHx1] [m^-3]
+%   latitude                 - Latitude of the measurment station [1x1]
+%   longitude                - Longitude of the measurement station [1x1]
+%   time                     - Date-time measurments in matlab units
+%   mode            - 0: uses electronDensity as input
+%                              1: uses IRI2016 Ne as input</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% GW - A struct array containing the following parameters
+%      datenum,ByIMF,BzIMF,Velocity_SW,Density_P,Pressure_dynamic,G:[G1 G2 G3]  
+%      Status8, kp,akp3,dst,Bz1_6:[Bz1,Bz2,Bz3,Bz4,Bz5,Bz6],W:[W1 W2 W3 W4 W5 W6]
+%      Status6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D47" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% yyyy -     [yyyy] An integer indicating the year for which you would like
+%             to calculate G &amp; W.
+%           
+% programDir - A string indicating the directory where the program 
+%              MagmodelinputONE.exe is. Which is compiled using g77 from 
+%              MagmodelinputONE.f manually.
+%              Default: '~\github\energy-height-conversion\Tools\...
+%              External Tools\Tsyganenko_Parameters\MagParameterProgram-rsw\'
+% omniASCDir - The director where the ASC omni files will be downloaded by 
+%              download_omni_cdf(...,'asc');
+%              Default: '~\githun\LargeFiles\omni\ASC\'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1971,7 +2280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0" shapeId="0">
+    <comment ref="B51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2002,7 +2311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D43" authorId="0" shapeId="0">
+    <comment ref="D51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2033,7 +2342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0" shapeId="0">
+    <comment ref="B52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2059,7 +2368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D44" authorId="0" shapeId="0">
+    <comment ref="D52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2088,7 +2397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D45" authorId="0" shapeId="0">
+    <comment ref="D53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2117,7 +2426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0">
+    <comment ref="B54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2141,7 +2450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D46" authorId="0" shapeId="0">
+    <comment ref="D54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2176,7 +2485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0" shapeId="0">
+    <comment ref="B57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2200,7 +2509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="0" shapeId="0">
+    <comment ref="D57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2241,7 +2550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0" shapeId="0">
+    <comment ref="B60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2265,7 +2574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D49" authorId="0" shapeId="0">
+    <comment ref="D60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2300,7 +2609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="0" shapeId="0">
+    <comment ref="D61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2327,7 +2636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B51" authorId="0" shapeId="0">
+    <comment ref="B62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2352,7 +2661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2382,7 +2691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0" shapeId="0">
+    <comment ref="B63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2406,7 +2715,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="0" shapeId="0">
+    <comment ref="D63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2437,7 +2746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="0" shapeId="0">
+    <comment ref="D64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2463,7 +2772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="0" shapeId="0">
+    <comment ref="D71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2485,6 +2794,362 @@
           <t xml:space="preserve">
 % dataChoice - Array of numbers - each number associated with a data set 
 %              to be plotted in order</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B75" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% az          : Azimuth points rotated in the right direction (0 deg -&gt; North 
+%               and 90 -&gt; East)
+% el          : Elevation points after rotating [1-D Array] 
+% goodData    : Logic array, with all the good coordinates labeled 1, and
+%               bad coordinates (with an grad(az)&gt;15) labelled 0.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D75" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% azCal       : Azimuth Coordinate of data from cal file (Default form: 0 deg -&gt; West;
+%               90 deg -&gt; North [MxN Matrix]
+% elCal       : Elevation Coordinate of data from cal file [MxN Matrix]
+% imageSize   : The size to which you would like the FITS data to be
+%               interpolated to [Eg., 512]
+% dateCal     : The matlab datenum value of the calibration file</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D82" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+%   rawVoltages - [nSamples x nRanges x nPulsesPerRecord x nRecords]
+%   code        - phase code</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B83" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+%   C.info  - contains the name of the constant and units
+%   C.c     - speed of light`
+%   C.kb    - boltazmann constant
+%   C.e     - elementary charge
+%   C.epsilon0 - electric constant
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D84" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% dateStr   - 'dd mmm yyyy'; default : '26 Mar 2008'
+% storeDir  - Directory where the FITS files should be downloaded to
+%           - Default: '~\LargeFiles\DASC\'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D85" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% dataStr - [dd mmm yyyy] A string indicating date for which you would like
+%           to download the omni data
+%           Default:'26 Mar 2008'
+% storeDir- A string indicating the data storage directory in '...\github\'
+%           It will store the hourly data in ~\yyyymmdd\omni\hourly\
+%           and 1 min data in ~yyyymmdd\omni\1min\
+%           Default: '~\github\LargeFiles\'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B86" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Stores the cdf files in Store Dir</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D86" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% dataStr - [dd mmm yyyy] A string indicating date for which you would like
+%           to download the omni data
+%           Default:'26 Mar 2008'
+% storeDir- A string indicating the data storage directory in '...\github\'
+%           It will store the data into ~\themis\state\
+%           Default: '~\github\LargeFiles\'
+% probeStr- A string listing the themis probes you would like the data from
+%           Default: 'tha,thb,thc,thd,the' all of them
+% dataType- A string listing the instrument from which data is to be downloaded 
+%           'state', 'sst'  etc.
+%           Default: 'state' - which is position of the satellite</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D99" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nithin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% paths.fitsDirName -&gt; contains the folder with fits files
+% paths.imageDirName -&gt; the folder where the figures will be stored
+% timeLimStr.min -&gt; '01 Mar 2011 9:00:00'
+% timeLimStr.max -&gt; '01 Mar 2011 10:00:00'
+% latLim -&gt; [63 67]
+% DASCcalFile.az - azimuth calibration file of DASC
+% DASCcalFile.el - elevation calibration file of DASC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B100" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% isThereNAN : A boolean variable, True =&gt; there is nan values in the
+%                   array, and False =&gt; there is no nan values in the array
+% totalNAN   : The total number of NAN values</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D100" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% thisArray : An array or a matrix</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B103" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% rootPathStr - A string containg git directory path in the present computer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D104" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nithin Sivadas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+% figureHandle
+% vert - Vertical page size in mm (Default Letter Size)
+% horz - Horizontal page size in mm (Default Letter Size)
+</t>
         </r>
       </text>
     </comment>
@@ -2493,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="384">
   <si>
     <t>Folder</t>
   </si>
@@ -3124,6 +3789,552 @@
   </si>
   <si>
     <t>Integrates beam-wise conductivity along altitude</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>data -&gt; electronDensity, altitude, range, time, 
+dNeFrac, site.latitude,
+site.longitude, site.altitude, magBeamNo, nBeams, az, el</t>
+  </si>
+  <si>
+    <t>read_amisr</t>
+  </si>
+  <si>
+    <t>fileNameStr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reads the specific data in h5 format obtained from amisr.com datasets. </t>
+  </si>
+  <si>
+    <t>magBeamNo</t>
+  </si>
+  <si>
+    <t>find_field_aligned_beam_no</t>
+  </si>
+  <si>
+    <t>beamCodes, magFieldAlignedAz, magFieldAlignedElev</t>
+  </si>
+  <si>
+    <t>Finds the field aligned beam number given the
+field aligned Az and Elev values, using the beamCodes matrix from SRI-AMISR data sets</t>
+  </si>
+  <si>
+    <t>flag, probeNames</t>
+  </si>
+  <si>
+    <t>find_geodetic_conjunction</t>
+  </si>
+  <si>
+    <t>probes, conjunctionCoords, stropAlt</t>
+  </si>
+  <si>
+    <t>Calculates conjunction between geodetic coordinates at stopAlt height</t>
+  </si>
+  <si>
+    <t>probes</t>
+  </si>
+  <si>
+    <t>find_magnetic_conjunctions</t>
+  </si>
+  <si>
+    <t>time, omniData, spacecraft, groundstation, conjunction, stopAlt, hemiFlag, magFieldModel</t>
+  </si>
+  <si>
+    <t>Calculates magnetic conjunction between spacecraft, groundstation and selected conjunction probe at stopAlt heights</t>
+  </si>
+  <si>
+    <t>get_2D_energy_spectra</t>
+  </si>
+  <si>
+    <t>amisrData,energyBin,
+timeMinStr,timeMaxStr,
+altLim,setTypeofCoords</t>
+  </si>
+  <si>
+    <t>dataInv,coords,inputInv</t>
+  </si>
+  <si>
+    <t>Converts electron density to energy spectra and prepares a  struct variable which can be used to plot 2D energy flux slices</t>
+  </si>
+  <si>
+    <t>noiseDist, signalDist, dopplerShiftDist, fWidthDist</t>
+  </si>
+  <si>
+    <t>get_ACF_parameter_distribution_1</t>
+  </si>
+  <si>
+    <t>nSamples,nPulseTrains,
+nExperiments,noisePower,
+signalPower,
+dopplerFrequency,fWidth,
+sampleTime</t>
+  </si>
+  <si>
+    <t>Runs a monte-carlo simulation to estimate the statistical distribution of singal,noise, doppler-shifted frequency and spectra width from a modelled stochastic ISR signal with an underlying probability distribution. The probability distribution is gaussian with zero mean and an autocorrelation function modelled with parameters specified by noisePower, signalPower, dopplerFrequency, fWidth.</t>
+  </si>
+  <si>
+    <t>get_DASC_filename</t>
+  </si>
+  <si>
+    <t>fileStrName</t>
+  </si>
+  <si>
+    <t>dirName, timeStr</t>
+  </si>
+  <si>
+    <t>Identifies the file closest to the specified time
+in 'timeStr'</t>
+  </si>
+  <si>
+    <t>get_amisr_experiment_times</t>
+  </si>
+  <si>
+    <t>table, tableHeader</t>
+  </si>
+  <si>
+    <t>timeMinStr, timeMaxStr, instrumentID</t>
+  </si>
+  <si>
+    <t>Scrapes experiment details from amisr website</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alt, electronDensity, latitude, longitude, time, mode</t>
+  </si>
+  <si>
+    <t>outputArguments -&gt; sigma_P, sigma_H, alt</t>
+  </si>
+  <si>
+    <t>get_conductivity_v1</t>
+  </si>
+  <si>
+    <t>Returns the hall and pederson conductivity given an input electron density value, along with some other output parameters.</t>
+  </si>
+  <si>
+    <t>get_fft</t>
+  </si>
+  <si>
+    <t>x,sampleTime,mode</t>
+  </si>
+  <si>
+    <t>S,f</t>
+  </si>
+  <si>
+    <t>FFT of x(t) with t&gt;=0 to generate S(f)</t>
+  </si>
+  <si>
+    <t>get_files_in_folders</t>
+  </si>
+  <si>
+    <t>dirName, wildcard</t>
+  </si>
+  <si>
+    <t>fileStr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produces a cell array of all file names in folder </t>
+  </si>
+  <si>
+    <t>get_power_spectra</t>
+  </si>
+  <si>
+    <t>x,t,mode</t>
+  </si>
+  <si>
+    <t>S,f,moments</t>
+  </si>
+  <si>
+    <t>Calculate power spectra with input signal or ACF</t>
+  </si>
+  <si>
+    <t>get_tsyganenko_GW_1</t>
+  </si>
+  <si>
+    <t>yyyy,programDir,omniASCDir</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>Runs the fortran code MagParametersProgramONE to calculate G1-G3, and W1-W6: input parameters to the tsyganenko magnetic field models 2001, 2003.</t>
+  </si>
+  <si>
+    <t>interpolate_to_field_aligned_coords</t>
+  </si>
+  <si>
+    <t>amisrData, timeMinStr, timeMaxStr</t>
+  </si>
+  <si>
+    <t>amisrData</t>
+  </si>
+  <si>
+    <t>figureHandle</t>
+  </si>
+  <si>
+    <t>Interpolate origCartCoords &amp; electronDensity to specified magCartCoords &amp; magElectronDensity</t>
+  </si>
+  <si>
+    <t>DASC_aer_to_geodetic_v2018</t>
+  </si>
+  <si>
+    <t>calculate_peak_altitude_of_ionization</t>
+  </si>
+  <si>
+    <t>calibrate_DASC_pixels</t>
+  </si>
+  <si>
+    <t>create_DASC_hdf5</t>
+  </si>
+  <si>
+    <t>create_DASC_hdf5_low_memory</t>
+  </si>
+  <si>
+    <t>create_amisr_web_experiment_H5_database</t>
+  </si>
+  <si>
+    <t>create_energyFlux_hdf5</t>
+  </si>
+  <si>
+    <t>create_energy_spectra_images</t>
+  </si>
+  <si>
+    <t>create_omni_HDF5</t>
+  </si>
+  <si>
+    <t>decoding</t>
+  </si>
+  <si>
+    <t>define_universal_constants</t>
+  </si>
+  <si>
+    <t>download_DASC_FITS</t>
+  </si>
+  <si>
+    <t>download_omni_cdf</t>
+  </si>
+  <si>
+    <t>download_themis</t>
+  </si>
+  <si>
+    <t>find_magnetic_conjunctions_at_mag_equator</t>
+  </si>
+  <si>
+    <t>generate_energy_spectra_data_product</t>
+  </si>
+  <si>
+    <t>geodetic_distance</t>
+  </si>
+  <si>
+    <t>get_free_mem</t>
+  </si>
+  <si>
+    <t>get_kpap</t>
+  </si>
+  <si>
+    <t>h5read_data</t>
+  </si>
+  <si>
+    <t>integrate_pulses</t>
+  </si>
+  <si>
+    <t>msis_irbem</t>
+  </si>
+  <si>
+    <t>process_omni_data</t>
+  </si>
+  <si>
+    <t>process_themis_data</t>
+  </si>
+  <si>
+    <t>read_DASC_fits</t>
+  </si>
+  <si>
+    <t>reshape_beam_wise</t>
+  </si>
+  <si>
+    <t>store_2D_energy_slice_with_DASC</t>
+  </si>
+  <si>
+    <t>goodDataMinElRemoved, lat, lon, alt</t>
+  </si>
+  <si>
+    <t>az, el, minElevation, projectionAltitude, sensorLoc</t>
+  </si>
+  <si>
+    <t>Converts input Digital All Sky Camera image with az, el coordinates to lat, lon projected at the given projection altitude.</t>
+  </si>
+  <si>
+    <t>energy,time0,lat,lon,alt</t>
+  </si>
+  <si>
+    <t>peakIonizationAlt</t>
+  </si>
+  <si>
+    <t>Calculated the peak ionization altitude using the Segienko &amp; Ivanov 1993 model of electron precipitation and MSIS00</t>
+  </si>
+  <si>
+    <t>azCal,elCal,imageSize,dateCal</t>
+  </si>
+  <si>
+    <t>az, el, goodData</t>
+  </si>
+  <si>
+    <t>Use data from calibration FIT files to calculate the az, el of each pixel - as well as cut off bad data with large az gradients.</t>
+  </si>
+  <si>
+    <t>localStoreDir,outputH5FileStr,projectionAltitude,
+minElevation, minTimeStr, maxTimeStr, calFileAz, calFileEl, setDownloadDASCFlag</t>
+  </si>
+  <si>
+    <t>dataASILastDay</t>
+  </si>
+  <si>
+    <t>localStoreDir,outputH5FileStr,    projectionAltitudeDASC,
+minElevation,minTimeStr,
+maxTimeStr,calFileAz,
+calFileEl, setDownloadDASCFlag</t>
+  </si>
+  <si>
+    <t>timeMinStr,timeMaxStr,instrumentID,outputH5File,writeModeStr</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dataStructure,amisrMagDataStructure,h5FileStr,mode</t>
+  </si>
+  <si>
+    <t>h5FileStr, imageStoreDir, videoFileNameStr, energySlice, eFluxLim,  opticalLim,  timeMinStr, timeMaxStr, latLim, lonLim, setStoreImage</t>
+  </si>
+  <si>
+    <t>time, timePrimary</t>
+  </si>
+  <si>
+    <t>h5FileStr,localStorePath,setCalculateGW</t>
+  </si>
+  <si>
+    <t>data,status</t>
+  </si>
+  <si>
+    <t>rawVoltages,code</t>
+  </si>
+  <si>
+    <t>decodedSignal</t>
+  </si>
+  <si>
+    <t>Decoding a phase coded signal by matchfiltering it with the known phase-coded signal</t>
+  </si>
+  <si>
+    <t>Defining universal constants</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>dateStr,storeDir</t>
+  </si>
+  <si>
+    <t>status,cmdout</t>
+  </si>
+  <si>
+    <t>Downloads all PokerFlat DASC FITS file which are not already in storeDir</t>
+  </si>
+  <si>
+    <t>Downloads hourly and minute-wise omni values</t>
+  </si>
+  <si>
+    <t>dateStr,storeDir,dataType</t>
+  </si>
+  <si>
+    <t>dateStr,storeDir,probeStr,dataType</t>
+  </si>
+  <si>
+    <t>Downloads themis data (currently only state)</t>
+  </si>
+  <si>
+    <t>time, maginput,  spacecraft, conjunction, stopAlt,  hemiFlag, magFieldModel</t>
+  </si>
+  <si>
+    <t>Calculates magnetic conjunction between 
+spacecraft, groundstation and selected conjunction probe at stopAlt heights</t>
+  </si>
+  <si>
+    <t>amisrFileStr, amisrRootPath, dascRootPath,     projectionAltPFISR, projectionAltDASC, energyBin, altLim, outputH5FileStr,  timeMinStr, timeMaxStr,  dascMinElevation, dascCalFileAz, dascCalFileEl,  dascSetDownloadFlag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generates the energy spectra data product that contains the magnetically field aligned electron densities, energy flux of primary electrons that generate the aurora, and DASC camera data to put them in context. </t>
+  </si>
+  <si>
+    <t>coord1,coord2,radius</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shortest distance between two points in geodetic coordinates using Harversine formulae </t>
+  </si>
+  <si>
+    <t>Show free memory in linux</t>
+  </si>
+  <si>
+    <t>kpap,kpapHeader</t>
+  </si>
+  <si>
+    <t>Get KP, AP, and F10.7 Index from geophys parameters. Can be used for msis.</t>
+  </si>
+  <si>
+    <t>yearStr, setForceDownload, localStoreDir, url</t>
+  </si>
+  <si>
+    <t>h5FilePath</t>
+  </si>
+  <si>
+    <t>data, h5DataLoc</t>
+  </si>
+  <si>
+    <t>Reads all h5 data from an h5 file into a structure data</t>
+  </si>
+  <si>
+    <t>inputSignal, inputTime, nPulsesIntegrated</t>
+  </si>
+  <si>
+    <t>outputSignal, outputTime</t>
+  </si>
+  <si>
+    <t>Integrates the pulses of a decoded, and reshaped raw voltages for the number of pulses prescribed.</t>
+  </si>
+  <si>
+    <t>timeMSIS, coords, msisVersionStr, coordType</t>
+  </si>
+  <si>
+    <t>msisData, F107A, F107, APH</t>
+  </si>
+  <si>
+    <t>Wrapper for IRBEM MSIS, default version nrlmsise00</t>
+  </si>
+  <si>
+    <t>omniData, matFilePath</t>
+  </si>
+  <si>
+    <t>themisData, matFilePath</t>
+  </si>
+  <si>
+    <t>Processes hourly and minute-wise omni data and stores it as .mat files, under each event date folder. Can be used as input for magnetic field models through IRBEM</t>
+  </si>
+  <si>
+    <t>dateStr, dataStoreDir, setCalculateGW</t>
+  </si>
+  <si>
+    <t>dateStr, dataStoreDir, probeStr, dataType</t>
+  </si>
+  <si>
+    <t>Process and download themis state data for one month</t>
+  </si>
+  <si>
+    <t>fileNameStr,imageSize</t>
+  </si>
+  <si>
+    <t>imageData,time</t>
+  </si>
+  <si>
+    <t>Reading DASC FITS file, changing resolution, and extracting time stamp</t>
+  </si>
+  <si>
+    <t>Reshapes the inputSignal along beam-wise (careful)</t>
+  </si>
+  <si>
+    <t>outputSignal, uniqueBeamCodes, outputTime</t>
+  </si>
+  <si>
+    <t>inputSignal, beamCode, inputTime</t>
+  </si>
+  <si>
+    <t>paths, timeLimStr, DASCcalFile, latLim, lonLim, amisrData, dataInv, magcoords</t>
+  </si>
+  <si>
+    <t>Stores PFISR energy slice overlayed on Digital All-Sky Camera image as a png file in paths.imageDirName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates images of energy spectra overlaid on optical images from eneryFlux HDF5 file, and then stores the images on a folder specified by imageStore Dir. </t>
+  </si>
+  <si>
+    <t>plot_1D_time_slice_with_error</t>
+  </si>
+  <si>
+    <t>time, yAxis, zValue, zError, thisTime, mode</t>
+  </si>
+  <si>
+    <t>plot_2D_conductivity_slice_geodetic</t>
+  </si>
+  <si>
+    <t>data, geodeticCoords, timeNo, altitudeSelected, conductivityType, setMapOn, latLim, lonLim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plotting a 2D slice of PFISR conductivites</t>
+  </si>
+  <si>
+    <t>plot_2D_conductivity_slice_geodetic_faster</t>
+  </si>
+  <si>
+    <t>FscatteredInterpolant, geodeticCoords, altitudeSelected, setMapOn, latLim, lonLim</t>
+  </si>
+  <si>
+    <t>plot_2D_density_slice_geodetic</t>
+  </si>
+  <si>
+    <t>data, geodeticCoords, timeNo, altitudeSelected, setMapOn, latLim, lonLim</t>
+  </si>
+  <si>
+    <t>plot_2D_density_slice_geodetic_aer</t>
+  </si>
+  <si>
+    <t>data, geodeticCoords, altitude, nBeams, timeNo, altitudeSelected, setMapOn</t>
+  </si>
+  <si>
+    <t>plot_2D_energy_slice_geodetic_v1</t>
+  </si>
+  <si>
+    <t>data, amisrData, coords,     energyBin, nBeams, timeNo, altitude, energy, latWidth, lonWidth, setMapOn, setTimeLabelOn</t>
+  </si>
+  <si>
+    <t>Plot 2D differential energy flux slices from 4-D PFISR data sets on lat, long map</t>
+  </si>
+  <si>
+    <t>plot_2D_energy_slice_with_DASC</t>
+  </si>
+  <si>
+    <t>figureHandle, timeStr, dataInvEnergySpectra, amisrData, magcoords, DASCcalFile, DASCdataFolder, latLim, lonLim, storeImageDir</t>
+  </si>
+  <si>
+    <t>plot_2D_integrated_conductivity_map</t>
+  </si>
+  <si>
+    <t>data, mode, timeNo, setMapOn, latLim, lonLim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plotting a 2D map of integrated conductivity</t>
+  </si>
+  <si>
+    <t>create_magneticFieldProjection_hdf5</t>
+  </si>
+  <si>
+    <t>Creates HDF5 file with specified magnetic field parameters</t>
+  </si>
+  <si>
+    <t>magFieldModel, inputH5FileStr, omniH5FileStr</t>
+  </si>
+  <si>
+    <t>plot_2D_magnetic_foot_points</t>
+  </si>
+  <si>
+    <t>Given a matrix of magnetic conjugate points at the equatorial plane, and their corresponding ionospheric foot points, the function draws a contour plot of their equatorial radial distances.</t>
+  </si>
+  <si>
+    <t>magEqPointGEO, ionosphereCoord, BfieldModelStr, thisTimeBfieldModel, setMapOn, latLim, lonLim, contourArray, setFieldLabelOn, setTimeLabelOn, imageSize</t>
+  </si>
+  <si>
+    <t>h2, ax2</t>
   </si>
 </sst>
 </file>
@@ -3229,7 +4440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3263,6 +4474,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3391,7 +4608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3504,12 +4721,71 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3752,26 +5028,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0"/>
@@ -3788,18 +5044,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F99" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:F99"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Folder" dataDxfId="5"/>
-    <tableColumn id="2" name="Output" dataDxfId="4"/>
-    <tableColumn id="3" name="Function Name" dataDxfId="3"/>
-    <tableColumn id="4" name="Input" dataDxfId="2"/>
-    <tableColumn id="5" name="Description" dataDxfId="1"/>
-    <tableColumn id="6" name="Last Updated" dataDxfId="0"/>
+    <tableColumn id="1" name="Folder" dataDxfId="9"/>
+    <tableColumn id="2" name="Output" dataDxfId="8"/>
+    <tableColumn id="3" name="Function Name" dataDxfId="7"/>
+    <tableColumn id="4" name="Input" dataDxfId="6"/>
+    <tableColumn id="5" name="Description" dataDxfId="5"/>
+    <tableColumn id="6" name="Last Updated" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4068,10 +5324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4420,79 +5676,75 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>179</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F19" s="36"/>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C21" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="F18" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="18">
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="18">
-        <v>42760</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="F21" s="18">
         <v>42634</v>
@@ -4503,39 +5755,37 @@
         <v>180</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>39</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D22" s="16"/>
       <c r="E22" s="17" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F22" s="18">
-        <v>42638</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>42760</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F23" s="18">
-        <v>42635</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4543,99 +5793,99 @@
         <v>180</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F24" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F25" s="18">
         <v>42638</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>186</v>
+        <v>42</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="F26" s="18">
-        <v>42638</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>187</v>
+        <v>46</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>193</v>
+        <v>47</v>
       </c>
       <c r="F27" s="18">
-        <v>42638</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>177</v>
+        <v>50</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="F28" s="18">
-        <v>42773</v>
+        <v>42638</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4643,19 +5893,19 @@
         <v>180</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F29" s="18">
-        <v>42759</v>
+        <v>42638</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4663,434 +5913,414 @@
         <v>180</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>75</v>
+        <v>193</v>
       </c>
       <c r="F30" s="18">
-        <v>42657</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>42638</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F31" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>42773</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F32" s="18">
-        <v>42634</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>54</v>
+        <v>182</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="F33" s="18">
-        <v>42774</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>42657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>58</v>
+        <v>178</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="F34" s="18">
         <v>42634</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>63</v>
+        <v>78</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>183</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F35" s="18">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="18">
+        <v>42774</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="18">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="18">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="22"/>
+      <c r="B39" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="36"/>
+    </row>
+    <row r="40" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F40" s="36"/>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F41" s="36"/>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="22"/>
+      <c r="B42" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="F42" s="36"/>
+    </row>
+    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="22"/>
+      <c r="B43" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="F43" s="36"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="22"/>
+      <c r="B44" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="F44" s="36"/>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="22"/>
+      <c r="B45" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="F45" s="36"/>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="22"/>
+      <c r="B46" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="F46" s="36"/>
+    </row>
+    <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A47" s="22"/>
+      <c r="B47" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F47" s="36"/>
+    </row>
+    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="22"/>
+      <c r="B48" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F48" s="36"/>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C49" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D49" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E49" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="F36" s="36">
+      <c r="F49" s="36">
         <v>42927</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="18">
-        <v>42635</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F38" s="19"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="19"/>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F40" s="18">
-        <v>42776</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F41" s="19"/>
-    </row>
-    <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="F44" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="F45" s="18">
-        <v>42642</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="F46" s="18">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F47" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F48" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" s="18">
-        <v>42658</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="15" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="F50" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="F51" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="F52" s="18">
         <v>42759</v>
@@ -5102,45 +6332,940 @@
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F53" s="18">
+        <v>42642</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F54" s="18">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="25"/>
+      <c r="B55" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="E55" s="17"/>
+      <c r="F55" s="18"/>
+    </row>
+    <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F56" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F57" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A58" s="25"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="F58" s="18">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="25"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="18"/>
+    </row>
+    <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F60" s="18">
+        <v>42658</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F61" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F62" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F63" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B64" s="14"/>
+      <c r="C64" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D64" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E64" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="F53" s="18">
+      <c r="F64" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="26" t="s">
+    <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="25"/>
+      <c r="B65" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="F65" s="18"/>
+    </row>
+    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="25"/>
+      <c r="B66" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="E66" s="17"/>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="25"/>
+      <c r="B67" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="F67" s="18"/>
+    </row>
+    <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="25"/>
+      <c r="B68" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="E68" s="17"/>
+      <c r="F68" s="18"/>
+    </row>
+    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="25"/>
+      <c r="B69" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="E69" s="17"/>
+      <c r="F69" s="18"/>
+    </row>
+    <row r="70" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="25"/>
+      <c r="B70" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="F70" s="18">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="28" t="s">
+      <c r="B71" s="27"/>
+      <c r="C71" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D71" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="E71" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="F54" s="31">
+      <c r="F71" s="31">
         <v>42759</v>
       </c>
     </row>
+    <row r="72" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C72" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="D72" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="F72" s="42"/>
+    </row>
+    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73" s="39" t="s">
+        <v>292</v>
+      </c>
+      <c r="C73" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="D73" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="F73" s="42"/>
+    </row>
+    <row r="74" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="C74" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="D74" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="F74" s="42"/>
+    </row>
+    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="C75" s="40" t="s">
+        <v>267</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="F75" s="43">
+        <v>43238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="C76" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="E76" s="30"/>
+      <c r="F76" s="42"/>
+    </row>
+    <row r="77" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="C77" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="E77" s="30"/>
+      <c r="F77" s="42"/>
+    </row>
+    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="C78" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="E78" s="30"/>
+      <c r="F78" s="42"/>
+    </row>
+    <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="E79" s="30"/>
+      <c r="F79" s="42"/>
+    </row>
+    <row r="80" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="C80" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="D80" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="F80" s="42"/>
+      <c r="G80" s="44"/>
+    </row>
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B81" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="C81" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="E81" s="30"/>
+      <c r="F81" s="42"/>
+    </row>
+    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="C82" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="F82" s="42"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="C83" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D83" s="41"/>
+      <c r="E83" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="F83" s="42"/>
+    </row>
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="C84" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="F84" s="42"/>
+    </row>
+    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" s="39"/>
+      <c r="C85" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="F85" s="42"/>
+    </row>
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B86" s="39"/>
+      <c r="C86" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="F86" s="42"/>
+    </row>
+    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C87" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="F87" s="42"/>
+    </row>
+    <row r="88" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A88" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="C88" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="F88" s="42"/>
+    </row>
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="C89" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="E89" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="F89" s="42"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B90" s="39"/>
+      <c r="C90" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="D90" s="41"/>
+      <c r="E90" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="F90" s="42"/>
+    </row>
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A91" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="C91" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="F91" s="42"/>
+    </row>
+    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="C92" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="F92" s="42"/>
+    </row>
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A93" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="C93" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="D93" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="E93" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="F93" s="42"/>
+    </row>
+    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="C94" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="E94" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="F94" s="42"/>
+    </row>
+    <row r="95" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="C95" s="40" t="s">
+        <v>287</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="E95" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="F95" s="42"/>
+    </row>
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="C96" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="E96" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="F96" s="42"/>
+    </row>
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A97" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C97" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="F97" s="42"/>
+    </row>
+    <row r="98" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="C98" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="F98" s="42"/>
+    </row>
+    <row r="99" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="39"/>
+      <c r="C99" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="F99" s="42"/>
+    </row>
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F100" s="18">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B101" s="14"/>
+      <c r="C101" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E101" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F101" s="19"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B102" s="14"/>
+      <c r="C102" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E102" s="17"/>
+      <c r="F102" s="19"/>
+    </row>
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D103" s="16"/>
+      <c r="E103" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F103" s="18">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B104" s="14"/>
+      <c r="C104" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E104" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F104" s="19"/>
+    </row>
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="F105" s="18">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B106" s="14"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="16"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C10 C12:C1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+  <conditionalFormatting sqref="C81:C1048576 C21:C72 C1:C10 C12:C17">
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73:C80">
+    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1"/>
+    <hyperlink ref="C38" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>

</xml_diff>

<commit_message>
Done with combine_2D_plot.m and incorporated L-shells * L-star in create_magneticFieldProjection_hdf5.m
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -2772,7 +2772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D71" authorId="0" shapeId="0">
+    <comment ref="D74" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2797,7 +2797,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="1" shapeId="0">
+    <comment ref="B78" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2825,7 +2825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D75" authorId="1" shapeId="0">
+    <comment ref="D78" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2854,7 +2854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D82" authorId="1" shapeId="0">
+    <comment ref="D85" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="1" shapeId="0">
+    <comment ref="B86" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2908,7 +2908,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D84" authorId="1" shapeId="0">
+    <comment ref="D87" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2934,7 +2934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D85" authorId="1" shapeId="0">
+    <comment ref="D88" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2964,7 +2964,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="1" shapeId="0">
+    <comment ref="B89" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2988,7 +2988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D86" authorId="1" shapeId="0">
+    <comment ref="D89" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3022,7 +3022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D99" authorId="1" shapeId="0">
+    <comment ref="D102" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3052,7 +3052,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0" shapeId="0">
+    <comment ref="B103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3078,7 +3078,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D100" authorId="0" shapeId="0">
+    <comment ref="D103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3102,7 +3102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0" shapeId="0">
+    <comment ref="B106" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3126,7 +3126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D104" authorId="0" shapeId="0">
+    <comment ref="D107" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3158,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="390">
   <si>
     <t>Folder</t>
   </si>
@@ -4335,6 +4335,24 @@
   </si>
   <si>
     <t>h2, ax2</t>
+  </si>
+  <si>
+    <t>get_2D_plot_inputs_at_time</t>
+  </si>
+  <si>
+    <t>inputH5FileStr, plotModeStr, thisTimeIndx, magFieldModelStr</t>
+  </si>
+  <si>
+    <t>plotData</t>
+  </si>
+  <si>
+    <t>Get inputs required to plot at a particular time instant for HDF5 file</t>
+  </si>
+  <si>
+    <t>plot_2D_energy_slice_geodetic_v2018</t>
+  </si>
+  <si>
+    <t>get_2D_plot_inputs_time_independent</t>
   </si>
 </sst>
 </file>
@@ -5044,8 +5062,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F99" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:F99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F102" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:F102"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
@@ -5324,10 +5342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6542,7 +6560,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="25"/>
       <c r="B65" s="14" t="s">
         <v>263</v>
@@ -6558,7 +6576,7 @@
       </c>
       <c r="F65" s="18"/>
     </row>
-    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="25"/>
       <c r="B66" s="14" t="s">
         <v>263</v>
@@ -6572,7 +6590,7 @@
       <c r="E66" s="17"/>
       <c r="F66" s="18"/>
     </row>
-    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="25"/>
       <c r="B67" s="14" t="s">
         <v>263</v>
@@ -6588,7 +6606,7 @@
       </c>
       <c r="F67" s="18"/>
     </row>
-    <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="25"/>
       <c r="B68" s="14" t="s">
         <v>263</v>
@@ -6602,7 +6620,7 @@
       <c r="E68" s="17"/>
       <c r="F68" s="18"/>
     </row>
-    <row r="69" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="25"/>
       <c r="B69" s="14" t="s">
         <v>263</v>
@@ -6616,8 +6634,10 @@
       <c r="E69" s="17"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="25"/>
+    <row r="70" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="25" t="s">
+        <v>185</v>
+      </c>
       <c r="B70" s="14" t="s">
         <v>383</v>
       </c>
@@ -6634,454 +6654,436 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="26" t="s">
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="25"/>
+      <c r="B71" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="F71" s="18"/>
+    </row>
+    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A72" s="25"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="18"/>
+    </row>
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="25"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="18"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B71" s="27"/>
-      <c r="C71" s="28" t="s">
+      <c r="B74" s="27"/>
+      <c r="C74" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D74" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E74" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="F71" s="31">
+      <c r="F74" s="31">
         <v>42759</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="38" t="s">
+    <row r="75" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="B72" s="39" t="s">
+      <c r="B75" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="C72" s="40" t="s">
+      <c r="C75" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="D72" s="41" t="s">
+      <c r="D75" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="E72" s="30" t="s">
+      <c r="E75" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="F72" s="42"/>
-    </row>
-    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B73" s="39" t="s">
-        <v>292</v>
-      </c>
-      <c r="C73" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="D73" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="E73" s="30" t="s">
-        <v>294</v>
-      </c>
-      <c r="F73" s="42"/>
-    </row>
-    <row r="74" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B74" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="C74" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="D74" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="E74" s="30" t="s">
-        <v>297</v>
-      </c>
-      <c r="F74" s="42"/>
-    </row>
-    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B75" s="27" t="s">
-        <v>299</v>
-      </c>
-      <c r="C75" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="D75" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="E75" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="F75" s="43">
-        <v>43238</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F75" s="42"/>
+    </row>
+    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B76" s="27" t="s">
-        <v>302</v>
+      <c r="B76" s="39" t="s">
+        <v>292</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="D76" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="E76" s="30"/>
+        <v>265</v>
+      </c>
+      <c r="D76" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>294</v>
+      </c>
       <c r="F76" s="42"/>
     </row>
-    <row r="77" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="D77" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="E77" s="30"/>
+        <v>266</v>
+      </c>
+      <c r="D77" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>297</v>
+      </c>
       <c r="F77" s="42"/>
     </row>
-    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>304</v>
-      </c>
-      <c r="E78" s="30"/>
-      <c r="F78" s="42"/>
-    </row>
-    <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="F78" s="43">
+        <v>43238</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A79" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>29</v>
+        <v>302</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E79" s="30"/>
       <c r="F79" s="42"/>
     </row>
-    <row r="80" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="E80" s="30" t="s">
-        <v>357</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="E80" s="30"/>
       <c r="F80" s="42"/>
-      <c r="G80" s="44"/>
-    </row>
-    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E81" s="30"/>
       <c r="F81" s="42"/>
     </row>
-    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>312</v>
+        <v>29</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>313</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="E82" s="30"/>
       <c r="F82" s="42"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="C83" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="D83" s="41"/>
+        <v>308</v>
+      </c>
+      <c r="C83" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="D83" s="29" t="s">
+        <v>307</v>
+      </c>
       <c r="E83" s="30" t="s">
-        <v>314</v>
+        <v>357</v>
       </c>
       <c r="F83" s="42"/>
-    </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G83" s="44"/>
+    </row>
+    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>317</v>
-      </c>
-      <c r="C84" s="28" t="s">
-        <v>276</v>
+        <v>310</v>
+      </c>
+      <c r="C84" s="40" t="s">
+        <v>273</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="E84" s="30" t="s">
-        <v>318</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="E84" s="30"/>
       <c r="F84" s="42"/>
     </row>
-    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B85" s="39"/>
+      <c r="B85" s="27" t="s">
+        <v>312</v>
+      </c>
       <c r="C85" s="40" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B86" s="39"/>
-      <c r="C86" s="40" t="s">
-        <v>278</v>
-      </c>
-      <c r="D86" s="29" t="s">
-        <v>321</v>
-      </c>
+      <c r="B86" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D86" s="41"/>
       <c r="E86" s="30" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F86" s="42"/>
     </row>
-    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>220</v>
+        <v>317</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="F87" s="42"/>
     </row>
-    <row r="88" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B88" s="27" t="s">
-        <v>305</v>
-      </c>
+      <c r="B88" s="39"/>
       <c r="C88" s="40" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D88" s="29" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E88" s="30" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F88" s="42"/>
     </row>
-    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B89" s="27" t="s">
-        <v>328</v>
-      </c>
+      <c r="B89" s="39"/>
       <c r="C89" s="40" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D89" s="29" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="F89" s="42"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B90" s="39"/>
-      <c r="C90" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="D90" s="41"/>
+      <c r="B90" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="D90" s="29" t="s">
+        <v>323</v>
+      </c>
       <c r="E90" s="30" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="F90" s="42"/>
     </row>
-    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A91" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="C91" s="40" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="F91" s="42"/>
     </row>
-    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C92" s="40" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E92" s="30" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F92" s="42"/>
     </row>
-    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B93" s="27" t="s">
-        <v>338</v>
-      </c>
+      <c r="B93" s="39"/>
       <c r="C93" s="40" t="s">
-        <v>285</v>
-      </c>
-      <c r="D93" s="29" t="s">
-        <v>337</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D93" s="41"/>
       <c r="E93" s="30" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F93" s="42"/>
     </row>
-    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C94" s="40" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="F94" s="42"/>
     </row>
-    <row r="95" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C95" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="F95" s="42"/>
     </row>
-    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C96" s="40" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="F96" s="42"/>
     </row>
@@ -7090,50 +7092,52 @@
         <v>190</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="C97" s="28" t="s">
-        <v>289</v>
+        <v>341</v>
+      </c>
+      <c r="C97" s="40" t="s">
+        <v>286</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="F97" s="42"/>
     </row>
-    <row r="98" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C98" s="40" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="F98" s="42"/>
     </row>
-    <row r="99" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B99" s="39"/>
+      <c r="B99" s="27" t="s">
+        <v>344</v>
+      </c>
       <c r="C99" s="40" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F99" s="42"/>
     </row>
@@ -7141,118 +7145,170 @@
       <c r="A100" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B100" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D100" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F100" s="18">
-        <v>42635</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B100" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C100" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="D100" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="F100" s="42"/>
+    </row>
+    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B101" s="14"/>
-      <c r="C101" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E101" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F101" s="19"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B101" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="C101" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="D101" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="E101" s="30" t="s">
+        <v>352</v>
+      </c>
+      <c r="F101" s="42"/>
+    </row>
+    <row r="102" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B102" s="14"/>
-      <c r="C102" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E102" s="17"/>
-      <c r="F102" s="19"/>
+      <c r="B102" s="39"/>
+      <c r="C102" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="D102" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="E102" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="F102" s="42"/>
     </row>
     <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D103" s="16"/>
+        <v>131</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="E103" s="17" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="F103" s="18">
-        <v>42776</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B104" s="14"/>
-      <c r="C104" s="15" t="s">
-        <v>171</v>
+      <c r="C104" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="F104" s="19"/>
     </row>
-    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B105" s="14" t="s">
-        <v>305</v>
-      </c>
+      <c r="B105" s="14"/>
       <c r="C105" s="15" t="s">
-        <v>377</v>
+        <v>144</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="E105" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="F105" s="18">
-        <v>43373</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="E105" s="17"/>
+      <c r="F105" s="19"/>
+    </row>
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B106" s="14"/>
-      <c r="C106" s="15"/>
+      <c r="B106" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="D106" s="16"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="19"/>
+      <c r="E106" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F106" s="18">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" s="14"/>
+      <c r="C107" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E107" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F107" s="19"/>
+    </row>
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A108" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="E108" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="F108" s="18">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B109" s="14"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C81:C1048576 C21:C72 C1:C10 C12:C17">
+  <conditionalFormatting sqref="C84:C1048576 C21:C75 C1:C10 C12:C17">
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
@@ -7261,7 +7317,7 @@
   <conditionalFormatting sqref="C18:C20">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73:C80">
+  <conditionalFormatting sqref="C76:C83">
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Added functionality to plot L, and Lstar in combine_plot_2D.m
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -3158,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="392">
   <si>
     <t>Folder</t>
   </si>
@@ -4353,6 +4353,12 @@
   </si>
   <si>
     <t>get_2D_plot_inputs_time_independent</t>
+  </si>
+  <si>
+    <t>combine_2D_plots</t>
+  </si>
+  <si>
+    <t>Plot optical images, energy flux maps, and or magnetic field maps over one another.</t>
   </si>
 </sst>
 </file>
@@ -5344,8 +5350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7297,15 +7303,23 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B109" s="14"/>
-      <c r="C109" s="15"/>
+      <c r="B109" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>390</v>
+      </c>
       <c r="D109" s="16"/>
-      <c r="E109" s="17"/>
-      <c r="F109" s="19"/>
+      <c r="E109" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="F109" s="18">
+        <v>43378</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C84:C1048576 C21:C75 C1:C10 C12:C17">

</xml_diff>

<commit_message>
can plot ration of Rc wrt gyro-radius, and hence visualize the isotropic boundary of electrons
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="17280" windowHeight="4104"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="17280" windowHeight="4110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2249,7 +2249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="0" shapeId="0">
+    <comment ref="D51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2280,7 +2280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B51" authorId="0" shapeId="0">
+    <comment ref="B52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2311,7 +2311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2342,7 +2342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0" shapeId="0">
+    <comment ref="B53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2368,7 +2368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="0" shapeId="0">
+    <comment ref="D53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2397,7 +2397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="0" shapeId="0">
+    <comment ref="D54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2426,7 +2426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B54" authorId="0" shapeId="0">
+    <comment ref="B55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2450,7 +2450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="0" shapeId="0">
+    <comment ref="D55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2485,7 +2485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B57" authorId="0" shapeId="0">
+    <comment ref="B58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2509,7 +2509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D57" authorId="0" shapeId="0">
+    <comment ref="D58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2550,7 +2550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B60" authorId="0" shapeId="0">
+    <comment ref="B61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2574,7 +2574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D60" authorId="0" shapeId="0">
+    <comment ref="D61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2609,7 +2609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D61" authorId="0" shapeId="0">
+    <comment ref="D62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2636,7 +2636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0" shapeId="0">
+    <comment ref="B63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2661,7 +2661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D62" authorId="0" shapeId="0">
+    <comment ref="D63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2691,7 +2691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B63" authorId="0" shapeId="0">
+    <comment ref="B64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2715,7 +2715,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D63" authorId="0" shapeId="0">
+    <comment ref="D64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2746,7 +2746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D64" authorId="0" shapeId="0">
+    <comment ref="D65" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2772,7 +2772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D74" authorId="0" shapeId="0">
+    <comment ref="D75" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2797,7 +2797,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B78" authorId="1" shapeId="0">
+    <comment ref="B79" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2825,7 +2825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D78" authorId="1" shapeId="0">
+    <comment ref="D79" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2854,7 +2854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D85" authorId="1" shapeId="0">
+    <comment ref="D86" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="1" shapeId="0">
+    <comment ref="B87" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2908,7 +2908,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D87" authorId="1" shapeId="0">
+    <comment ref="D88" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2934,7 +2934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D88" authorId="1" shapeId="0">
+    <comment ref="D89" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2964,7 +2964,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B89" authorId="1" shapeId="0">
+    <comment ref="B90" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2988,7 +2988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D89" authorId="1" shapeId="0">
+    <comment ref="D90" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3022,7 +3022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D102" authorId="1" shapeId="0">
+    <comment ref="D103" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3052,7 +3052,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0" shapeId="0">
+    <comment ref="B104" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3078,7 +3078,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D103" authorId="0" shapeId="0">
+    <comment ref="D104" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3102,7 +3102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0" shapeId="0">
+    <comment ref="B107" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3126,7 +3126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D107" authorId="0" shapeId="0">
+    <comment ref="D108" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3158,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="393">
   <si>
     <t>Folder</t>
   </si>
@@ -4359,6 +4359,9 @@
   </si>
   <si>
     <t>Plot optical images, energy flux maps, and or magnetic field maps over one another.</t>
+  </si>
+  <si>
+    <t>get_isotropic_boundary</t>
   </si>
 </sst>
 </file>
@@ -5068,8 +5071,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F102" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:F102"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F103" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:F103"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
@@ -5348,23 +5351,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="20.21875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="20.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="38.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5384,7 +5387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>79</v>
       </c>
@@ -5404,7 +5407,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -5422,7 +5425,7 @@
       </c>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>79</v>
       </c>
@@ -5442,7 +5445,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>79</v>
       </c>
@@ -5462,7 +5465,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>79</v>
       </c>
@@ -5482,7 +5485,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -5502,7 +5505,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>79</v>
       </c>
@@ -5522,7 +5525,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>79</v>
       </c>
@@ -5542,7 +5545,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>79</v>
       </c>
@@ -5562,7 +5565,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="14" t="s">
         <v>195</v>
@@ -5580,7 +5583,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>79</v>
       </c>
@@ -5600,7 +5603,7 @@
         <v>42635</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>79</v>
       </c>
@@ -5620,7 +5623,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>79</v>
       </c>
@@ -5640,7 +5643,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>79</v>
       </c>
@@ -5660,7 +5663,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>179</v>
       </c>
@@ -5680,7 +5683,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>179</v>
       </c>
@@ -5700,7 +5703,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>179</v>
       </c>
@@ -5718,7 +5721,7 @@
       </c>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>179</v>
       </c>
@@ -5736,7 +5739,7 @@
       </c>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>179</v>
       </c>
@@ -5754,7 +5757,7 @@
       </c>
       <c r="F20" s="36"/>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>179</v>
       </c>
@@ -5774,7 +5777,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>180</v>
       </c>
@@ -5792,7 +5795,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>180</v>
       </c>
@@ -5812,7 +5815,7 @@
         <v>42760</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>180</v>
       </c>
@@ -5832,7 +5835,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>180</v>
       </c>
@@ -5852,7 +5855,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>180</v>
       </c>
@@ -5872,7 +5875,7 @@
         <v>42635</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>180</v>
       </c>
@@ -5892,7 +5895,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>180</v>
       </c>
@@ -5912,7 +5915,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>180</v>
       </c>
@@ -5932,7 +5935,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>180</v>
       </c>
@@ -5952,7 +5955,7 @@
         <v>42638</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>180</v>
       </c>
@@ -5972,7 +5975,7 @@
         <v>42773</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>180</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>180</v>
       </c>
@@ -6012,7 +6015,7 @@
         <v>42657</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>180</v>
       </c>
@@ -6032,7 +6035,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>180</v>
       </c>
@@ -6052,7 +6055,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>180</v>
       </c>
@@ -6072,7 +6075,7 @@
         <v>42774</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>180</v>
       </c>
@@ -6092,7 +6095,7 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>180</v>
       </c>
@@ -6112,7 +6115,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
       <c r="B39" s="33" t="s">
         <v>226</v>
@@ -6128,7 +6131,7 @@
       </c>
       <c r="F39" s="36"/>
     </row>
-    <row r="40" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="33" t="s">
         <v>228</v>
@@ -6144,7 +6147,7 @@
       </c>
       <c r="F40" s="36"/>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
       <c r="B41" s="33" t="s">
         <v>233</v>
@@ -6160,7 +6163,7 @@
       </c>
       <c r="F41" s="36"/>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="33" t="s">
         <v>237</v>
@@ -6176,7 +6179,7 @@
       </c>
       <c r="F42" s="36"/>
     </row>
-    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
       <c r="B43" s="33" t="s">
         <v>241</v>
@@ -6192,7 +6195,7 @@
       </c>
       <c r="F43" s="36"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
       <c r="B44" s="33" t="s">
         <v>246</v>
@@ -6208,7 +6211,7 @@
       </c>
       <c r="F44" s="36"/>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="33" t="s">
         <v>250</v>
@@ -6224,7 +6227,7 @@
       </c>
       <c r="F45" s="36"/>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
       <c r="B46" s="33" t="s">
         <v>254</v>
@@ -6240,7 +6243,7 @@
       </c>
       <c r="F46" s="36"/>
     </row>
-    <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
       <c r="B47" s="33" t="s">
         <v>258</v>
@@ -6256,7 +6259,7 @@
       </c>
       <c r="F47" s="36"/>
     </row>
-    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
       <c r="B48" s="33" t="s">
         <v>262</v>
@@ -6272,157 +6275,147 @@
       </c>
       <c r="F48" s="36"/>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="22" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="D49" s="35"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="36"/>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B49" s="33" t="s">
+      <c r="B50" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C50" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D50" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E50" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="F49" s="36">
+      <c r="F50" s="36">
         <v>42927</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F50" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B51" s="14" t="s">
-        <v>135</v>
-      </c>
+      <c r="B51" s="14"/>
       <c r="C51" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F51" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F52" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="14"/>
+      <c r="B53" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="C53" s="15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F53" s="18">
-        <v>42642</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="14" t="s">
-        <v>150</v>
-      </c>
+      <c r="B54" s="14"/>
       <c r="C54" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F54" s="18">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="25"/>
+        <v>42642</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
+        <v>185</v>
+      </c>
       <c r="B55" s="14" t="s">
         <v>150</v>
       </c>
       <c r="C55" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F55" s="18">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="25"/>
+      <c r="B56" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D56" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="18"/>
-    </row>
-    <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F56" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E56" s="17"/>
+      <c r="F56" s="18"/>
+    </row>
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>185</v>
       </c>
@@ -6430,381 +6423,385 @@
         <v>72</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F57" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" s="25"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15" t="s">
-        <v>369</v>
+    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>370</v>
+        <v>71</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>371</v>
+        <v>176</v>
       </c>
       <c r="F58" s="18">
-        <v>43133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="25"/>
       <c r="B59" s="14"/>
       <c r="C59" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="F59" s="18">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="25"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D60" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="18"/>
-    </row>
-    <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F60" s="18">
-        <v>42658</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E60" s="17"/>
+      <c r="F60" s="18"/>
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="14"/>
+      <c r="B61" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C61" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F61" s="18">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>42658</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="B62" s="14"/>
       <c r="C62" s="15" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="F62" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="F63" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B64" s="14"/>
+      <c r="B64" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C64" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F64" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="25"/>
-      <c r="B65" s="14" t="s">
-        <v>263</v>
-      </c>
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="14"/>
       <c r="C65" s="15" t="s">
-        <v>360</v>
+        <v>163</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>361</v>
+        <v>164</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>362</v>
-      </c>
-      <c r="F65" s="18"/>
-    </row>
-    <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="F65" s="18">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="25"/>
       <c r="B66" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="E66" s="17"/>
+        <v>361</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>362</v>
+      </c>
       <c r="F66" s="18"/>
     </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="25"/>
       <c r="B67" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>376</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="E67" s="17"/>
       <c r="F67" s="18"/>
     </row>
-    <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="25"/>
       <c r="B68" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="E68" s="17"/>
+        <v>375</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>376</v>
+      </c>
       <c r="F68" s="18"/>
     </row>
-    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E69" s="17"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="25" t="s">
+    <row r="70" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="25"/>
+      <c r="B70" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="E70" s="17"/>
+      <c r="F70" s="18"/>
+    </row>
+    <row r="71" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A71" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B71" s="14" t="s">
         <v>383</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C71" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D71" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E71" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="F70" s="18">
+      <c r="F71" s="18">
         <v>43373</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="25"/>
-      <c r="B71" s="14" t="s">
+    <row r="72" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="25"/>
+      <c r="B72" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C72" s="15" t="s">
         <v>384</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D72" s="16" t="s">
         <v>385</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E72" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="F71" s="18"/>
-    </row>
-    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="25"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="17"/>
       <c r="F72" s="18"/>
     </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="14"/>
       <c r="C73" s="15" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D73" s="16"/>
       <c r="E73" s="17"/>
       <c r="F73" s="18"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="26" t="s">
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="25"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="18"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B74" s="27"/>
-      <c r="C74" s="28" t="s">
+      <c r="B75" s="27"/>
+      <c r="C75" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D74" s="29" t="s">
+      <c r="D75" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="E74" s="30" t="s">
+      <c r="E75" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="F74" s="31">
+      <c r="F75" s="31">
         <v>42759</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="38" t="s">
+    <row r="76" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A76" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="B75" s="39" t="s">
+      <c r="B76" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="C75" s="40" t="s">
+      <c r="C76" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="D75" s="41" t="s">
+      <c r="D76" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="E75" s="30" t="s">
+      <c r="E76" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="F75" s="42"/>
-    </row>
-    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B76" s="39" t="s">
-        <v>292</v>
-      </c>
-      <c r="C76" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="D76" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>294</v>
-      </c>
       <c r="F76" s="42"/>
     </row>
-    <row r="77" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B77" s="27" t="s">
-        <v>296</v>
+      <c r="B77" s="39" t="s">
+        <v>292</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D77" s="41" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F77" s="42"/>
     </row>
-    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="D78" s="29" t="s">
-        <v>298</v>
+        <v>266</v>
+      </c>
+      <c r="D78" s="41" t="s">
+        <v>295</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="F78" s="43">
-        <v>43238</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+      <c r="F78" s="42"/>
+    </row>
+    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="E79" s="30"/>
-      <c r="F79" s="42"/>
-    </row>
-    <row r="80" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="F79" s="43">
+        <v>43238</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
         <v>190</v>
       </c>
@@ -6812,517 +6809,533 @@
         <v>302</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E80" s="30"/>
       <c r="F80" s="42"/>
     </row>
-    <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E81" s="30"/>
       <c r="F81" s="42"/>
     </row>
-    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>29</v>
+        <v>305</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E82" s="30"/>
       <c r="F82" s="42"/>
     </row>
-    <row r="83" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>308</v>
+        <v>29</v>
       </c>
       <c r="C83" s="40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>357</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="E83" s="30"/>
       <c r="F83" s="42"/>
-      <c r="G83" s="44"/>
-    </row>
-    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C84" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="E84" s="30"/>
+        <v>307</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>357</v>
+      </c>
       <c r="F84" s="42"/>
-    </row>
-    <row r="85" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G84" s="44"/>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>313</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="E85" s="30"/>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="C86" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="D86" s="41"/>
+        <v>312</v>
+      </c>
+      <c r="C86" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>311</v>
+      </c>
       <c r="E86" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F86" s="42"/>
     </row>
-    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="D87" s="29" t="s">
-        <v>316</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D87" s="41"/>
       <c r="E87" s="30" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F87" s="42"/>
     </row>
-    <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B88" s="39"/>
-      <c r="C88" s="40" t="s">
-        <v>277</v>
+      <c r="B88" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="C88" s="28" t="s">
+        <v>276</v>
       </c>
       <c r="D88" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E88" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F88" s="42"/>
     </row>
-    <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B89" s="39"/>
       <c r="C89" s="40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D89" s="29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F89" s="42"/>
     </row>
-    <row r="90" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B90" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" s="28" t="s">
-        <v>279</v>
+      <c r="B90" s="39"/>
+      <c r="C90" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F90" s="42"/>
     </row>
-    <row r="91" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="C91" s="40" t="s">
-        <v>280</v>
+        <v>220</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>279</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F91" s="42"/>
     </row>
-    <row r="92" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="C92" s="40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E92" s="30" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F92" s="42"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B93" s="39"/>
+      <c r="B93" s="27" t="s">
+        <v>328</v>
+      </c>
       <c r="C93" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="D93" s="41"/>
+        <v>281</v>
+      </c>
+      <c r="D93" s="29" t="s">
+        <v>327</v>
+      </c>
       <c r="E93" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F93" s="42"/>
     </row>
-    <row r="94" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B94" s="27" t="s">
-        <v>331</v>
-      </c>
+      <c r="B94" s="39"/>
       <c r="C94" s="40" t="s">
-        <v>283</v>
-      </c>
-      <c r="D94" s="29" t="s">
-        <v>333</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D94" s="41"/>
       <c r="E94" s="30" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F94" s="42"/>
     </row>
-    <row r="95" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C95" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F95" s="42"/>
     </row>
-    <row r="96" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C96" s="40" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F96" s="42"/>
     </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C97" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F97" s="42"/>
     </row>
-    <row r="98" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C98" s="40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F98" s="42"/>
     </row>
-    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C99" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F99" s="42"/>
     </row>
-    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="C100" s="28" t="s">
-        <v>289</v>
+        <v>344</v>
+      </c>
+      <c r="C100" s="40" t="s">
+        <v>288</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F100" s="42"/>
     </row>
-    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>353</v>
-      </c>
-      <c r="C101" s="40" t="s">
-        <v>290</v>
+        <v>350</v>
+      </c>
+      <c r="C101" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F101" s="42"/>
     </row>
-    <row r="102" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B102" s="39"/>
+      <c r="B102" s="27" t="s">
+        <v>353</v>
+      </c>
       <c r="C102" s="40" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D102" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F102" s="42"/>
     </row>
-    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B103" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E103" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F103" s="18">
-        <v>42635</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B103" s="39"/>
+      <c r="C103" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="D103" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="E103" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="F103" s="42"/>
+    </row>
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B104" s="14"/>
-      <c r="C104" s="24" t="s">
-        <v>141</v>
+      <c r="B104" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F104" s="19"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="F104" s="18">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B105" s="14"/>
-      <c r="C105" s="15" t="s">
-        <v>144</v>
+      <c r="C105" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="D105" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E105" s="17"/>
+      <c r="E105" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="F105" s="19"/>
     </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B106" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="B106" s="14"/>
       <c r="C106" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D106" s="16"/>
-      <c r="E106" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F106" s="18">
-        <v>42776</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E106" s="17"/>
+      <c r="F106" s="19"/>
+    </row>
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B107" s="14"/>
+      <c r="B107" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="C107" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>170</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D107" s="16"/>
       <c r="E107" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F107" s="19"/>
-    </row>
-    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="F107" s="18">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B108" s="14" t="s">
-        <v>305</v>
-      </c>
+      <c r="B108" s="14"/>
       <c r="C108" s="15" t="s">
-        <v>377</v>
+        <v>171</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>379</v>
+        <v>170</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="F108" s="18">
-        <v>43373</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+      <c r="F108" s="19"/>
+    </row>
+    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B109" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="E109" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="F109" s="18">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B110" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C109" s="15" t="s">
+      <c r="C110" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="D109" s="16"/>
-      <c r="E109" s="17" t="s">
+      <c r="D110" s="16"/>
+      <c r="E110" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="F109" s="18">
+      <c r="F110" s="18">
         <v>43378</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C84:C1048576 C21:C75 C1:C10 C12:C17">
+  <conditionalFormatting sqref="C85:C1048576 C21:C76 C1:C10 C12:C17">
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
@@ -7331,7 +7344,7 @@
   <conditionalFormatting sqref="C18:C20">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76:C83">
+  <conditionalFormatting sqref="C77:C84">
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
pixel and energyflux comparison with change in pathdef
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="17280" windowHeight="4110"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="15525" windowHeight="1395"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2249,7 +2250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2280,7 +2281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0" shapeId="0">
+    <comment ref="B51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2311,7 +2312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="0" shapeId="0">
+    <comment ref="D51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2342,7 +2343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="0" shapeId="0">
+    <comment ref="B52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2368,7 +2369,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="0" shapeId="0">
+    <comment ref="D52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2397,7 +2398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="0" shapeId="0">
+    <comment ref="D53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2426,7 +2427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0" shapeId="0">
+    <comment ref="B54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2450,7 +2451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D55" authorId="0" shapeId="0">
+    <comment ref="D54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2485,7 +2486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B58" authorId="0" shapeId="0">
+    <comment ref="B57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2509,7 +2510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D58" authorId="0" shapeId="0">
+    <comment ref="D57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2550,7 +2551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="0" shapeId="0">
+    <comment ref="B60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2574,7 +2575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D61" authorId="0" shapeId="0">
+    <comment ref="D60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2609,7 +2610,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D62" authorId="0" shapeId="0">
+    <comment ref="D61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2636,7 +2637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B63" authorId="0" shapeId="0">
+    <comment ref="B62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2661,7 +2662,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D63" authorId="0" shapeId="0">
+    <comment ref="D62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2691,7 +2692,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B64" authorId="0" shapeId="0">
+    <comment ref="B63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2715,7 +2716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D64" authorId="0" shapeId="0">
+    <comment ref="D63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2746,7 +2747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D65" authorId="0" shapeId="0">
+    <comment ref="D64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2772,7 +2773,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D75" authorId="0" shapeId="0">
+    <comment ref="D74" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2797,7 +2798,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="1" shapeId="0">
+    <comment ref="B78" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2825,7 +2826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D79" authorId="1" shapeId="0">
+    <comment ref="D78" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2854,7 +2855,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D86" authorId="1" shapeId="0">
+    <comment ref="D85" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="1" shapeId="0">
+    <comment ref="B86" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2908,7 +2909,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D88" authorId="1" shapeId="0">
+    <comment ref="D87" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2934,7 +2935,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D89" authorId="1" shapeId="0">
+    <comment ref="D88" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2964,7 +2965,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B90" authorId="1" shapeId="0">
+    <comment ref="B89" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2988,7 +2989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D90" authorId="1" shapeId="0">
+    <comment ref="D89" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3022,7 +3023,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D103" authorId="1" shapeId="0">
+    <comment ref="D102" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3052,7 +3053,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0" shapeId="0">
+    <comment ref="B103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3078,7 +3079,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D104" authorId="0" shapeId="0">
+    <comment ref="D103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3102,7 +3103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0" shapeId="0">
+    <comment ref="B106" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3126,7 +3127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D108" authorId="0" shapeId="0">
+    <comment ref="D107" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3158,7 +3159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="392">
   <si>
     <t>Folder</t>
   </si>
@@ -4359,9 +4360,6 @@
   </si>
   <si>
     <t>Plot optical images, energy flux maps, and or magnetic field maps over one another.</t>
-  </si>
-  <si>
-    <t>get_isotropic_boundary</t>
   </si>
 </sst>
 </file>
@@ -4775,46 +4773,6 @@
   <dxfs count="14">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5055,6 +5013,46 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0"/>
@@ -5071,18 +5069,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F103" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:F103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F102" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F102"/>
   <sortState ref="A2:F51">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Folder" dataDxfId="9"/>
-    <tableColumn id="2" name="Output" dataDxfId="8"/>
-    <tableColumn id="3" name="Function Name" dataDxfId="7"/>
-    <tableColumn id="4" name="Input" dataDxfId="6"/>
-    <tableColumn id="5" name="Description" dataDxfId="5"/>
-    <tableColumn id="6" name="Last Updated" dataDxfId="4"/>
+    <tableColumn id="1" name="Folder" dataDxfId="5"/>
+    <tableColumn id="2" name="Output" dataDxfId="4"/>
+    <tableColumn id="3" name="Function Name" dataDxfId="3"/>
+    <tableColumn id="4" name="Input" dataDxfId="2"/>
+    <tableColumn id="5" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" name="Last Updated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5351,10 +5349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6275,69 +6273,79 @@
       </c>
       <c r="F48" s="36"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="33"/>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>200</v>
+      </c>
       <c r="C49" s="34" t="s">
-        <v>392</v>
-      </c>
-      <c r="D49" s="35"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="36"/>
-    </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="C50" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D49" s="35" t="s">
         <v>199</v>
       </c>
+      <c r="E49" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" s="36">
+        <v>42927</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="E50" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="F50" s="36">
-        <v>42927</v>
+        <v>126</v>
+      </c>
+      <c r="F50" s="18">
+        <v>42759</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B51" s="14"/>
+      <c r="B51" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="C51" s="15" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F51" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F52" s="18">
         <v>42759</v>
@@ -6347,73 +6355,73 @@
       <c r="A53" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="14" t="s">
-        <v>139</v>
-      </c>
+      <c r="B53" s="14"/>
       <c r="C53" s="15" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F53" s="18">
-        <v>42759</v>
+        <v>42642</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="14"/>
+      <c r="B54" s="14" t="s">
+        <v>150</v>
+      </c>
       <c r="C54" s="15" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F54" s="18">
-        <v>42642</v>
+        <v>42639</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
-        <v>185</v>
-      </c>
+      <c r="A55" s="25"/>
       <c r="B55" s="14" t="s">
         <v>150</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>149</v>
+        <v>358</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="F55" s="18">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
+        <v>359</v>
+      </c>
+      <c r="E55" s="17"/>
+      <c r="F55" s="18"/>
+    </row>
+    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
+        <v>185</v>
+      </c>
       <c r="B56" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>358</v>
+        <v>72</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>359</v>
-      </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="18"/>
+        <v>152</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F56" s="18">
+        <v>42759</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
@@ -6423,161 +6431,157 @@
         <v>72</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F57" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>194</v>
+    <row r="58" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58" s="25"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15" t="s">
+        <v>369</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>71</v>
+        <v>370</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>176</v>
+        <v>371</v>
       </c>
       <c r="F58" s="18">
-        <v>42759</v>
+        <v>43133</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="25"/>
       <c r="B59" s="14"/>
       <c r="C59" s="15" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="F59" s="18">
-        <v>43133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
-      <c r="B60" s="14"/>
+        <v>373</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="18"/>
+    </row>
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="C60" s="15" t="s">
-        <v>372</v>
+        <v>154</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>373</v>
-      </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="18"/>
-    </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F60" s="18">
+        <v>42658</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="14" t="s">
-        <v>156</v>
-      </c>
+      <c r="B61" s="14"/>
       <c r="C61" s="15" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F61" s="18">
-        <v>42658</v>
+        <v>42759</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B62" s="14"/>
+      <c r="B62" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="C62" s="15" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
       <c r="F62" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="F63" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B64" s="14" t="s">
-        <v>156</v>
-      </c>
+      <c r="B64" s="14"/>
       <c r="C64" s="15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F64" s="18">
         <v>42759</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B65" s="14"/>
+    <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="25"/>
+      <c r="B65" s="14" t="s">
+        <v>263</v>
+      </c>
       <c r="C65" s="15" t="s">
-        <v>163</v>
+        <v>360</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>164</v>
+        <v>361</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F65" s="18">
-        <v>42759</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="F65" s="18"/>
     </row>
     <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="25"/>
@@ -6585,223 +6589,223 @@
         <v>263</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>362</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="E66" s="17"/>
       <c r="F66" s="18"/>
     </row>
-    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="25"/>
       <c r="B67" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="E67" s="17"/>
+        <v>375</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>376</v>
+      </c>
       <c r="F67" s="18"/>
     </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="25"/>
       <c r="B68" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>376</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="E68" s="17"/>
       <c r="F68" s="18"/>
     </row>
-    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="14" t="s">
         <v>263</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E69" s="17"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+    <row r="70" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A70" s="25" t="s">
+        <v>185</v>
+      </c>
       <c r="B70" s="14" t="s">
-        <v>263</v>
+        <v>383</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="E70" s="17"/>
-      <c r="F70" s="18"/>
-    </row>
-    <row r="71" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="25" t="s">
-        <v>185</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="F70" s="18">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="25"/>
       <c r="B71" s="14" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="F71" s="18">
-        <v>43373</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="F71" s="18"/>
+    </row>
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
-      <c r="B72" s="14" t="s">
-        <v>386</v>
-      </c>
+      <c r="B72" s="14"/>
       <c r="C72" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>385</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>387</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
       <c r="F72" s="18"/>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="14"/>
       <c r="C73" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D73" s="16"/>
       <c r="E73" s="17"/>
       <c r="F73" s="18"/>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="15" t="s">
-        <v>388</v>
-      </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="18"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="26" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B75" s="27"/>
-      <c r="C75" s="28" t="s">
+      <c r="B74" s="27"/>
+      <c r="C74" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D74" s="29" t="s">
         <v>168</v>
       </c>
+      <c r="E74" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F74" s="31">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A75" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C75" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="D75" s="41" t="s">
+        <v>210</v>
+      </c>
       <c r="E75" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="F75" s="31">
-        <v>42759</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A76" s="38" t="s">
-        <v>207</v>
+        <v>211</v>
+      </c>
+      <c r="F75" s="42"/>
+    </row>
+    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>208</v>
+        <v>292</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
       <c r="D76" s="41" t="s">
-        <v>210</v>
+        <v>293</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>211</v>
+        <v>294</v>
       </c>
       <c r="F76" s="42"/>
     </row>
-    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B77" s="39" t="s">
-        <v>292</v>
+      <c r="B77" s="27" t="s">
+        <v>296</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D77" s="41" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="F77" s="42"/>
     </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="D78" s="41" t="s">
-        <v>295</v>
+        <v>267</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>298</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>297</v>
-      </c>
-      <c r="F78" s="42"/>
-    </row>
-    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="F78" s="43">
+        <v>43238</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="F79" s="43">
-        <v>43238</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="E79" s="30"/>
+      <c r="F79" s="42"/>
+    </row>
+    <row r="80" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
         <v>190</v>
       </c>
@@ -6809,26 +6813,26 @@
         <v>302</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E80" s="30"/>
       <c r="F80" s="42"/>
     </row>
-    <row r="81" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E81" s="30"/>
       <c r="F81" s="42"/>
@@ -6838,99 +6842,101 @@
         <v>190</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>305</v>
+        <v>29</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E82" s="30"/>
       <c r="F82" s="42"/>
     </row>
-    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>29</v>
+        <v>308</v>
       </c>
       <c r="C83" s="40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>306</v>
-      </c>
-      <c r="E83" s="30"/>
+        <v>307</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>357</v>
+      </c>
       <c r="F83" s="42"/>
-    </row>
-    <row r="84" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="G83" s="44"/>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C84" s="40" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="E84" s="30" t="s">
-        <v>357</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="E84" s="30"/>
       <c r="F84" s="42"/>
-      <c r="G84" s="44"/>
-    </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="E85" s="30"/>
+        <v>311</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>313</v>
+      </c>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>312</v>
-      </c>
-      <c r="C86" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="D86" s="29" t="s">
-        <v>311</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D86" s="41"/>
       <c r="E86" s="30" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F86" s="42"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="D87" s="41"/>
+        <v>276</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>316</v>
+      </c>
       <c r="E87" s="30" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="F87" s="42"/>
     </row>
@@ -6938,17 +6944,15 @@
       <c r="A88" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B88" s="27" t="s">
-        <v>317</v>
-      </c>
-      <c r="C88" s="28" t="s">
-        <v>276</v>
+      <c r="B88" s="39"/>
+      <c r="C88" s="40" t="s">
+        <v>277</v>
       </c>
       <c r="D88" s="29" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E88" s="30" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F88" s="42"/>
     </row>
@@ -6958,187 +6962,189 @@
       </c>
       <c r="B89" s="39"/>
       <c r="C89" s="40" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D89" s="29" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="F89" s="42"/>
     </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B90" s="39"/>
-      <c r="C90" s="40" t="s">
-        <v>278</v>
+      <c r="B90" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" s="28" t="s">
+        <v>279</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F90" s="42"/>
     </row>
-    <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A91" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="C91" s="28" t="s">
-        <v>279</v>
+        <v>305</v>
+      </c>
+      <c r="C91" s="40" t="s">
+        <v>280</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="F91" s="42"/>
     </row>
-    <row r="92" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="C92" s="40" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E92" s="30" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F92" s="42"/>
     </row>
-    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B93" s="27" t="s">
-        <v>328</v>
-      </c>
+      <c r="B93" s="39"/>
       <c r="C93" s="40" t="s">
-        <v>281</v>
-      </c>
-      <c r="D93" s="29" t="s">
-        <v>327</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D93" s="41"/>
       <c r="E93" s="30" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F93" s="42"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B94" s="39"/>
+      <c r="B94" s="27" t="s">
+        <v>331</v>
+      </c>
       <c r="C94" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="D94" s="41"/>
+        <v>283</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>333</v>
+      </c>
       <c r="E94" s="30" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F94" s="42"/>
     </row>
-    <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C95" s="40" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="F95" s="42"/>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C96" s="40" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F96" s="42"/>
     </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C97" s="40" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F97" s="42"/>
     </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C98" s="40" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="F98" s="42"/>
     </row>
-    <row r="99" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C99" s="40" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F99" s="42"/>
     </row>
@@ -7147,205 +7153,187 @@
         <v>190</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>344</v>
-      </c>
-      <c r="C100" s="40" t="s">
-        <v>288</v>
+        <v>350</v>
+      </c>
+      <c r="C100" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="F100" s="42"/>
     </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="C101" s="28" t="s">
-        <v>289</v>
+        <v>353</v>
+      </c>
+      <c r="C101" s="40" t="s">
+        <v>290</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F101" s="42"/>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B102" s="27" t="s">
-        <v>353</v>
-      </c>
+      <c r="B102" s="39"/>
       <c r="C102" s="40" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D102" s="29" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="F102" s="42"/>
     </row>
-    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B103" s="39"/>
-      <c r="C103" s="40" t="s">
-        <v>291</v>
-      </c>
-      <c r="D103" s="29" t="s">
-        <v>355</v>
-      </c>
-      <c r="E103" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="F103" s="42"/>
+      <c r="B103" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E103" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F103" s="18">
+        <v>42635</v>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B104" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>131</v>
+      <c r="B104" s="14"/>
+      <c r="C104" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F104" s="18">
-        <v>42635</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F104" s="19"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B105" s="14"/>
-      <c r="C105" s="24" t="s">
-        <v>141</v>
+      <c r="C105" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="D105" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E105" s="17" t="s">
-        <v>143</v>
-      </c>
+      <c r="E105" s="17"/>
       <c r="F105" s="19"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B106" s="14"/>
+      <c r="B106" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="C106" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D106" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E106" s="17"/>
-      <c r="F106" s="19"/>
-    </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="D106" s="16"/>
+      <c r="E106" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F106" s="18">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B107" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="B107" s="14"/>
       <c r="C107" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D107" s="16"/>
+        <v>171</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>170</v>
+      </c>
       <c r="E107" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F107" s="18">
-        <v>42776</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F107" s="19"/>
+    </row>
+    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B108" s="14"/>
+      <c r="B108" s="14" t="s">
+        <v>305</v>
+      </c>
       <c r="C108" s="15" t="s">
-        <v>171</v>
+        <v>377</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>170</v>
+        <v>379</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F108" s="19"/>
+        <v>378</v>
+      </c>
+      <c r="F108" s="18">
+        <v>43373</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="23" t="s">
         <v>190</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>305</v>
+        <v>150</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>379</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="D109" s="16"/>
       <c r="E109" s="17" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="F109" s="18">
-        <v>43373</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B110" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>390</v>
-      </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="F110" s="18">
         <v>43378</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C85:C1048576 C21:C76 C1:C10 C12:C17">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="C84:C1048576 C21:C75 C1:C10 C12:C17">
+    <cfRule type="duplicateValues" dxfId="13" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77:C84">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+  <conditionalFormatting sqref="C76:C83">
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C38" r:id="rId1"/>

</xml_diff>

<commit_message>
keogram and pixles comparison with energy flux
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -3159,7 +3159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="397">
   <si>
     <t>Folder</t>
   </si>
@@ -4360,6 +4360,21 @@
   </si>
   <si>
     <t>Plot optical images, energy flux maps, and or magnetic field maps over one another.</t>
+  </si>
+  <si>
+    <t>create_panels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figureHandle, 'totalPanelNo', 'panelSize', 'demargin',  'margintop', 'marginright', 'marginleft', </t>
+  </si>
+  <si>
+    <t>Creates a set of panels on a Letter Size page</t>
+  </si>
+  <si>
+    <t>create_keogram</t>
+  </si>
+  <si>
+    <t>keo,parallels</t>
   </si>
 </sst>
 </file>
@@ -5349,10 +5364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7320,6 +7335,28 @@
       </c>
       <c r="F109" s="18">
         <v>43378</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using geopack functions in a similar fashion to irbem
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="15525" windowHeight="1395"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="15528" windowHeight="1392"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3159,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="440">
   <si>
     <t>Folder</t>
   </si>
@@ -4466,6 +4465,45 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>combine_2D_plots_v2</t>
+  </si>
+  <si>
+    <t>add_ASI_background_to_hdf5</t>
+  </si>
+  <si>
+    <t>create_thm_hdf5</t>
+  </si>
+  <si>
+    <t>find_irbem_magneticFieldStr</t>
+  </si>
+  <si>
+    <t>find_irbem_magneticFieldNo</t>
+  </si>
+  <si>
+    <t>add_thm_hdf5</t>
+  </si>
+  <si>
+    <t>probeName, outputH5FileStr, omniH5FileStr</t>
+  </si>
+  <si>
+    <t>write_sc_to_hdf5</t>
+  </si>
+  <si>
+    <t>Write spacecraft state data to hdf5</t>
+  </si>
+  <si>
+    <t>h5OutputFile,probeName,time,XYZ_GEO,magFieldStr,NFoot,Lm</t>
+  </si>
+  <si>
+    <t>geopack_find_magequator</t>
+  </si>
+  <si>
+    <t>geopack_find_footpoint</t>
+  </si>
+  <si>
+    <t>geopack_find_curvature</t>
   </si>
 </sst>
 </file>
@@ -5467,24 +5505,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="20.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="20.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="45"/>
+    <col min="5" max="5" width="38.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5507,7 +5545,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>79</v>
       </c>
@@ -5530,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -5551,7 +5589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>79</v>
       </c>
@@ -5574,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>79</v>
       </c>
@@ -5597,7 +5635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>79</v>
       </c>
@@ -5620,7 +5658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -5643,7 +5681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>79</v>
       </c>
@@ -5666,7 +5704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>79</v>
       </c>
@@ -5689,7 +5727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>79</v>
       </c>
@@ -5712,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="14" t="s">
         <v>195</v>
@@ -5733,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>79</v>
       </c>
@@ -5756,7 +5794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>79</v>
       </c>
@@ -5779,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>79</v>
       </c>
@@ -5802,7 +5840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>79</v>
       </c>
@@ -5825,7 +5863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>179</v>
       </c>
@@ -5848,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>179</v>
       </c>
@@ -5871,7 +5909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>179</v>
       </c>
@@ -5892,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>179</v>
       </c>
@@ -5913,7 +5951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>179</v>
       </c>
@@ -5934,7 +5972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>179</v>
       </c>
@@ -5957,7 +5995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>180</v>
       </c>
@@ -5978,7 +6016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>180</v>
       </c>
@@ -6001,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>180</v>
       </c>
@@ -6024,7 +6062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>180</v>
       </c>
@@ -6047,7 +6085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>180</v>
       </c>
@@ -6070,7 +6108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>180</v>
       </c>
@@ -6093,7 +6131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>180</v>
       </c>
@@ -6116,7 +6154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>180</v>
       </c>
@@ -6139,7 +6177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>180</v>
       </c>
@@ -6162,7 +6200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>180</v>
       </c>
@@ -6185,7 +6223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>180</v>
       </c>
@@ -6208,7 +6246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>180</v>
       </c>
@@ -6231,7 +6269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>180</v>
       </c>
@@ -6254,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>180</v>
       </c>
@@ -6277,7 +6315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
         <v>180</v>
       </c>
@@ -6300,7 +6338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>180</v>
       </c>
@@ -6323,7 +6361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
         <v>180</v>
       </c>
@@ -6346,7 +6384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="33" t="s">
         <v>226</v>
@@ -6365,7 +6403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A40" s="22"/>
       <c r="B40" s="33" t="s">
         <v>228</v>
@@ -6384,7 +6422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
       <c r="B41" s="33" t="s">
         <v>233</v>
@@ -6403,7 +6441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="22"/>
       <c r="B42" s="33" t="s">
         <v>237</v>
@@ -6422,7 +6460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="22"/>
       <c r="B43" s="33" t="s">
         <v>241</v>
@@ -6441,7 +6479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="22"/>
       <c r="B44" s="33" t="s">
         <v>246</v>
@@ -6460,7 +6498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="22"/>
       <c r="B45" s="33" t="s">
         <v>250</v>
@@ -6479,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="22"/>
       <c r="B46" s="33" t="s">
         <v>254</v>
@@ -6498,7 +6536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="22"/>
       <c r="B47" s="33" t="s">
         <v>258</v>
@@ -6517,7 +6555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="22"/>
       <c r="B48" s="33" t="s">
         <v>262</v>
@@ -6536,7 +6574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="22" t="s">
         <v>180</v>
       </c>
@@ -6559,7 +6597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="25" t="s">
         <v>185</v>
       </c>
@@ -6580,7 +6618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>185</v>
       </c>
@@ -6603,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>185</v>
       </c>
@@ -6626,7 +6664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="25" t="s">
         <v>185</v>
       </c>
@@ -6647,7 +6685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="25" t="s">
         <v>185</v>
       </c>
@@ -6670,7 +6708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="25"/>
       <c r="B55" s="14" t="s">
         <v>150</v>
@@ -6687,7 +6725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
         <v>185</v>
       </c>
@@ -6710,7 +6748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="25" t="s">
         <v>185</v>
       </c>
@@ -6733,7 +6771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="25"/>
       <c r="B58" s="14"/>
       <c r="C58" s="15" t="s">
@@ -6752,7 +6790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="25"/>
       <c r="B59" s="14"/>
       <c r="C59" s="15" t="s">
@@ -6767,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>185</v>
       </c>
@@ -6787,7 +6825,7 @@
         <v>42658</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
         <v>185</v>
       </c>
@@ -6805,7 +6843,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
         <v>185</v>
       </c>
@@ -6825,7 +6863,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="25" t="s">
         <v>185</v>
       </c>
@@ -6845,7 +6883,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="25" t="s">
         <v>185</v>
       </c>
@@ -6863,7 +6901,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="25"/>
       <c r="B65" s="14" t="s">
         <v>263</v>
@@ -6879,7 +6917,7 @@
       </c>
       <c r="F65" s="18"/>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="25"/>
       <c r="B66" s="14" t="s">
         <v>263</v>
@@ -6893,7 +6931,7 @@
       <c r="E66" s="17"/>
       <c r="F66" s="18"/>
     </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="25"/>
       <c r="B67" s="14" t="s">
         <v>263</v>
@@ -6909,7 +6947,7 @@
       </c>
       <c r="F67" s="18"/>
     </row>
-    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="25"/>
       <c r="B68" s="14" t="s">
         <v>263</v>
@@ -6923,7 +6961,7 @@
       <c r="E68" s="17"/>
       <c r="F68" s="18"/>
     </row>
-    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="25"/>
       <c r="B69" s="14" t="s">
         <v>263</v>
@@ -6937,7 +6975,7 @@
       <c r="E69" s="17"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
         <v>185</v>
       </c>
@@ -6957,7 +6995,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
       <c r="B71" s="14" t="s">
         <v>386</v>
@@ -6973,7 +7011,7 @@
       </c>
       <c r="F71" s="18"/>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="25"/>
       <c r="B72" s="14"/>
       <c r="C72" s="15" t="s">
@@ -6983,7 +7021,7 @@
       <c r="E72" s="17"/>
       <c r="F72" s="18"/>
     </row>
-    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="25"/>
       <c r="B73" s="14"/>
       <c r="C73" s="15" t="s">
@@ -6993,7 +7031,7 @@
       <c r="E73" s="17"/>
       <c r="F73" s="18"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="26" t="s">
         <v>185</v>
       </c>
@@ -7011,7 +7049,7 @@
         <v>42759</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A75" s="38" t="s">
         <v>207</v>
       </c>
@@ -7029,7 +7067,7 @@
       </c>
       <c r="F75" s="42"/>
     </row>
-    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="23" t="s">
         <v>190</v>
       </c>
@@ -7047,7 +7085,7 @@
       </c>
       <c r="F76" s="42"/>
     </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="23" t="s">
         <v>190</v>
       </c>
@@ -7065,7 +7103,7 @@
       </c>
       <c r="F77" s="42"/>
     </row>
-    <row r="78" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="23" t="s">
         <v>190</v>
       </c>
@@ -7085,7 +7123,7 @@
         <v>43238</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A79" s="23" t="s">
         <v>190</v>
       </c>
@@ -7101,7 +7139,7 @@
       <c r="E79" s="30"/>
       <c r="F79" s="42"/>
     </row>
-    <row r="80" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" s="23" t="s">
         <v>190</v>
       </c>
@@ -7117,7 +7155,7 @@
       <c r="E80" s="30"/>
       <c r="F80" s="42"/>
     </row>
-    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="23" t="s">
         <v>190</v>
       </c>
@@ -7133,7 +7171,7 @@
       <c r="E81" s="30"/>
       <c r="F81" s="42"/>
     </row>
-    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="23" t="s">
         <v>190</v>
       </c>
@@ -7149,7 +7187,7 @@
       <c r="E82" s="30"/>
       <c r="F82" s="42"/>
     </row>
-    <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="23" t="s">
         <v>190</v>
       </c>
@@ -7168,7 +7206,7 @@
       <c r="F83" s="42"/>
       <c r="G83" s="46"/>
     </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="23" t="s">
         <v>190</v>
       </c>
@@ -7184,7 +7222,7 @@
       <c r="E84" s="30"/>
       <c r="F84" s="42"/>
     </row>
-    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="23" t="s">
         <v>190</v>
       </c>
@@ -7202,7 +7240,7 @@
       </c>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="23" t="s">
         <v>190</v>
       </c>
@@ -7218,7 +7256,7 @@
       </c>
       <c r="F86" s="42"/>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="23" t="s">
         <v>190</v>
       </c>
@@ -7236,7 +7274,7 @@
       </c>
       <c r="F87" s="42"/>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="23" t="s">
         <v>190</v>
       </c>
@@ -7252,7 +7290,7 @@
       </c>
       <c r="F88" s="42"/>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="23" t="s">
         <v>190</v>
       </c>
@@ -7268,7 +7306,7 @@
       </c>
       <c r="F89" s="42"/>
     </row>
-    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="23" t="s">
         <v>190</v>
       </c>
@@ -7286,7 +7324,7 @@
       </c>
       <c r="F90" s="42"/>
     </row>
-    <row r="91" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A91" s="23" t="s">
         <v>190</v>
       </c>
@@ -7304,7 +7342,7 @@
       </c>
       <c r="F91" s="42"/>
     </row>
-    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="23" t="s">
         <v>190</v>
       </c>
@@ -7322,7 +7360,7 @@
       </c>
       <c r="F92" s="42"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="23" t="s">
         <v>190</v>
       </c>
@@ -7336,7 +7374,7 @@
       </c>
       <c r="F93" s="42"/>
     </row>
-    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="23" t="s">
         <v>190</v>
       </c>
@@ -7354,7 +7392,7 @@
       </c>
       <c r="F94" s="42"/>
     </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="23" t="s">
         <v>190</v>
       </c>
@@ -7372,7 +7410,7 @@
       </c>
       <c r="F95" s="42"/>
     </row>
-    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="23" t="s">
         <v>190</v>
       </c>
@@ -7390,7 +7428,7 @@
       </c>
       <c r="F96" s="42"/>
     </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="23" t="s">
         <v>190</v>
       </c>
@@ -7408,7 +7446,7 @@
       </c>
       <c r="F97" s="42"/>
     </row>
-    <row r="98" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="23" t="s">
         <v>190</v>
       </c>
@@ -7426,7 +7464,7 @@
       </c>
       <c r="F98" s="42"/>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="23" t="s">
         <v>190</v>
       </c>
@@ -7444,7 +7482,7 @@
       </c>
       <c r="F99" s="42"/>
     </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="23" t="s">
         <v>190</v>
       </c>
@@ -7462,7 +7500,7 @@
       </c>
       <c r="F100" s="42"/>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" s="23" t="s">
         <v>190</v>
       </c>
@@ -7480,7 +7518,7 @@
       </c>
       <c r="F101" s="42"/>
     </row>
-    <row r="102" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>190</v>
       </c>
@@ -7496,7 +7534,7 @@
       </c>
       <c r="F102" s="42"/>
     </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
         <v>190</v>
       </c>
@@ -7516,7 +7554,7 @@
         <v>42635</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
         <v>190</v>
       </c>
@@ -7532,7 +7570,7 @@
       </c>
       <c r="F104" s="19"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="23" t="s">
         <v>190</v>
       </c>
@@ -7546,7 +7584,7 @@
       <c r="E105" s="17"/>
       <c r="F105" s="19"/>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="23" t="s">
         <v>190</v>
       </c>
@@ -7564,7 +7602,7 @@
         <v>42776</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="23" t="s">
         <v>190</v>
       </c>
@@ -7580,7 +7618,7 @@
       </c>
       <c r="F107" s="19"/>
     </row>
-    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="23" t="s">
         <v>190</v>
       </c>
@@ -7600,7 +7638,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="23" t="s">
         <v>190</v>
       </c>
@@ -7618,7 +7656,7 @@
         <v>43378</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B110" s="5" t="s">
         <v>150</v>
       </c>
@@ -7632,7 +7670,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B111" s="5" t="s">
         <v>396</v>
       </c>
@@ -7640,7 +7678,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B112" s="5" t="s">
         <v>400</v>
       </c>
@@ -7654,7 +7692,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="113" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B113" s="5" t="s">
         <v>403</v>
       </c>
@@ -7668,7 +7706,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="114" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B114" s="5" t="s">
         <v>408</v>
       </c>
@@ -7682,7 +7720,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="115" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
         <v>29</v>
       </c>
@@ -7696,7 +7734,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="116" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B116" s="5" t="s">
         <v>414</v>
       </c>
@@ -7710,7 +7748,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="117" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B117" s="5" t="s">
         <v>417</v>
       </c>
@@ -7724,7 +7762,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="118" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B118" s="5" t="s">
         <v>305</v>
       </c>
@@ -7738,7 +7776,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="119" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B119" s="5" t="s">
         <v>424</v>
       </c>
@@ -7750,6 +7788,65 @@
       </c>
       <c r="E119" s="3" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C120" s="4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C121" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C122" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C123" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C124" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C125" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C126" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C127" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C128" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C129" s="4" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trace field lines incorporates min energy being scattered due to violation of first adiabatic invariant
</commit_message>
<xml_diff>
--- a/Tools/Function_Descriptions.xlsx
+++ b/Tools/Function_Descriptions.xlsx
@@ -3158,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="442">
   <si>
     <t>Folder</t>
   </si>
@@ -4504,6 +4504,12 @@
   </si>
   <si>
     <t>geopack_find_curvature</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>extract_pad_toshi</t>
   </si>
 </sst>
 </file>
@@ -5505,7 +5511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C130" sqref="C130"/>
@@ -7844,9 +7850,17 @@
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C129" s="4" t="s">
         <v>439</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>